<commit_message>
Player attack & Attack animaion / Monster move & Attack animation
1. 플레이어 공격 모션(실 적용 안됨)
2. 몬스터 네비 매쉬로 이동 처리
3. 범위 내에 들어오면 공격
</commit_message>
<xml_diff>
--- a/기능구현서.xlsx
+++ b/기능구현서.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KGA\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KGA\Documents\GitHub\3D_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
   <si>
     <t>구현 내용</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -98,10 +98,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>몬스터 개체 단위 구현</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>몬스터 몹 팩 단위 구현</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -187,17 +183,49 @@
   </si>
   <si>
     <t>플레이어 이동 애니메이션</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>플레이어각 보는 방향에 따라 블랜드 트리 제작</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>기본 공격 애니메이션 콤보 만들기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>공격중엔 이동과 회전이 불가능하게 만들기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>몬스터 개체 애니메이션</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>몬스터 공격</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>몬스터가 특정 범위내에 플래이어가 있다면 
+플레이어를 따라오도록 네비게이션 시스템</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이슈 1) 네비 매시에서 거리를 구하는 방법이 있긴 한데, 어느 정도 거리가 멀면 infinity가 뜨는 문제가 발생 
+-&gt; 이동 거리에 따른 이동 처리 불가
+해결) 이동 경로에 있는 코너에 경로들을 더하는 메서드를 따로 제작해 거리를 구함</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이슈 1) 몬스터의 공격 애니메이션 관리를 트리거로 받아서 하고 있었는데, 트리거가 선입력 되는 문제 발생
+해결) 애니메이션 보간 때문에 트랜지션 상태에서 선입력이 발생. 보간을 꺼줬음</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>월드 좌표랑 카메라가 바라보는 좌표가 상이해 플레이어가 보는 방향에 따라 이동하는 문제가 발생
 - 때문에 이동 방향을 로컬 좌표가 아닌 월드 좌표로 컨버팅해서 문제를 해결
-이후 좌표계 변환은 완료 되었으나, 이동 벡터의 값이 정규화되지 않았음. 문제 해결 요함
+이후 좌표계 변환은 완료 되었으나, 이동 벡터의 값이 정규화되지 않았음. 
 - 월드 좌표로 컨버팅 하는 과정에서 카메라 좌표의 Y축 값이 섞여 있어 좌표계가 찌그러 지는 현상이 있었음. Y좌표값을 0으로 바꿔주므로써 해결</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>플레이어각 보는 방향에 따라 블랜드 트리 제작</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -299,7 +327,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -340,6 +368,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -629,10 +666,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C5:J31"/>
+  <dimension ref="C5:J34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -640,18 +677,18 @@
     <col min="3" max="3" width="15.875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="48.75" style="1" customWidth="1"/>
     <col min="5" max="5" width="9" style="1"/>
-    <col min="6" max="6" width="62.5" style="1" customWidth="1"/>
+    <col min="6" max="6" width="69.125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="3:10">
       <c r="H5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I5" t="s">
+        <v>34</v>
+      </c>
+      <c r="J5" t="s">
         <v>35</v>
-      </c>
-      <c r="J5" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="6" spans="3:10">
@@ -672,7 +709,7 @@
       <c r="J6" s="11"/>
     </row>
     <row r="7" spans="3:10">
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="14" t="s">
         <v>7</v>
       </c>
       <c r="D7" s="8" t="s">
@@ -684,9 +721,9 @@
       <c r="F7" s="3"/>
     </row>
     <row r="8" spans="3:10">
-      <c r="C8" s="4"/>
+      <c r="C8" s="14"/>
       <c r="D8" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E8" s="9">
         <v>1</v>
@@ -694,7 +731,7 @@
       <c r="F8" s="3"/>
     </row>
     <row r="9" spans="3:10">
-      <c r="C9" s="4"/>
+      <c r="C9" s="14"/>
       <c r="D9" s="5" t="s">
         <v>6</v>
       </c>
@@ -703,22 +740,22 @@
       </c>
       <c r="F9" s="3"/>
     </row>
-    <row r="10" spans="3:10" ht="148.5">
-      <c r="C10" s="4"/>
+    <row r="10" spans="3:10" ht="115.5">
+      <c r="C10" s="14"/>
       <c r="D10" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E10" s="12">
         <v>1</v>
       </c>
       <c r="F10" s="13" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="3:10">
-      <c r="C11" s="4"/>
+      <c r="C11" s="14"/>
       <c r="D11" s="12" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E11" s="12">
         <v>1</v>
@@ -726,51 +763,53 @@
       <c r="F11" s="13"/>
     </row>
     <row r="12" spans="3:10">
-      <c r="C12" s="4"/>
-      <c r="D12" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="E12" s="5">
+      <c r="C12" s="14"/>
+      <c r="D12" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" s="12">
         <v>1</v>
       </c>
       <c r="F12" s="3"/>
     </row>
     <row r="13" spans="3:10">
-      <c r="C13" s="4"/>
-      <c r="D13" s="6" t="s">
+      <c r="C13" s="14"/>
+      <c r="D13" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E13" s="5">
+        <v>3</v>
+      </c>
+      <c r="F13" s="4"/>
+    </row>
+    <row r="14" spans="3:10">
+      <c r="C14" s="14"/>
+      <c r="D14" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="E13" s="5">
+      <c r="E14" s="12">
         <v>1</v>
       </c>
-      <c r="F13" s="3"/>
-    </row>
-    <row r="14" spans="3:10">
-      <c r="C14" s="4"/>
-      <c r="D14" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="E14" s="5">
+      <c r="F14" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="3:10">
+      <c r="C15" s="14"/>
+      <c r="D15" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E15" s="5">
         <v>8</v>
       </c>
-      <c r="F14" s="3"/>
-    </row>
-    <row r="15" spans="3:10">
-      <c r="C15" s="4" t="s">
+      <c r="F15" s="3"/>
+    </row>
+    <row r="16" spans="3:10">
+      <c r="C16" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D16" s="5" t="s">
         <v>10</v>
-      </c>
-      <c r="E15" s="5">
-        <v>3</v>
-      </c>
-      <c r="F15" s="3"/>
-    </row>
-    <row r="16" spans="3:10">
-      <c r="C16" s="4"/>
-      <c r="D16" s="5" t="s">
-        <v>11</v>
       </c>
       <c r="E16" s="5">
         <v>3</v>
@@ -778,9 +817,9 @@
       <c r="F16" s="3"/>
     </row>
     <row r="17" spans="3:6">
-      <c r="C17" s="4"/>
+      <c r="C17" s="14"/>
       <c r="D17" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E17" s="5">
         <v>3</v>
@@ -788,9 +827,9 @@
       <c r="F17" s="3"/>
     </row>
     <row r="18" spans="3:6">
-      <c r="C18" s="4"/>
+      <c r="C18" s="14"/>
       <c r="D18" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E18" s="5">
         <v>3</v>
@@ -798,21 +837,21 @@
       <c r="F18" s="3"/>
     </row>
     <row r="19" spans="3:6">
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="14"/>
+      <c r="D19" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E19" s="5">
+        <v>3</v>
+      </c>
+      <c r="F19" s="3"/>
+    </row>
+    <row r="20" spans="3:6">
+      <c r="C20" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="D20" s="5" t="s">
         <v>15</v>
-      </c>
-      <c r="E19" s="5">
-        <v>7</v>
-      </c>
-      <c r="F19" s="3"/>
-    </row>
-    <row r="20" spans="3:6">
-      <c r="C20" s="4"/>
-      <c r="D20" s="5" t="s">
-        <v>14</v>
       </c>
       <c r="E20" s="5">
         <v>7</v>
@@ -820,135 +859,169 @@
       <c r="F20" s="3"/>
     </row>
     <row r="21" spans="3:6">
-      <c r="C21" s="4" t="s">
+      <c r="C21" s="14"/>
+      <c r="D21" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E21" s="5">
+        <v>7</v>
+      </c>
+      <c r="F21" s="3"/>
+    </row>
+    <row r="22" spans="3:6" ht="66">
+      <c r="C22" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="E22" s="12">
+        <v>2</v>
+      </c>
+      <c r="F22" s="13" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" spans="3:6" ht="82.5">
+      <c r="C23" s="14"/>
+      <c r="D23" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="E23" s="12">
+        <v>2</v>
+      </c>
+      <c r="F23" s="13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24" spans="3:6">
+      <c r="C24" s="14"/>
+      <c r="D24" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="E24" s="15">
+        <v>2</v>
+      </c>
+      <c r="F24" s="4"/>
+    </row>
+    <row r="25" spans="3:6">
+      <c r="C25" s="14"/>
+      <c r="D25" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E25" s="5">
+        <v>2</v>
+      </c>
+      <c r="F25" s="3"/>
+    </row>
+    <row r="26" spans="3:6">
+      <c r="C26" s="14"/>
+      <c r="D26" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E26" s="5">
+        <v>4</v>
+      </c>
+      <c r="F26" s="3"/>
+    </row>
+    <row r="27" spans="3:6">
+      <c r="C27" s="14"/>
+      <c r="D27" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E27" s="5">
+        <v>4</v>
+      </c>
+      <c r="F27" s="3"/>
+    </row>
+    <row r="28" spans="3:6">
+      <c r="C28" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="D21" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E21" s="5">
-        <v>2</v>
-      </c>
-      <c r="F21" s="3"/>
-    </row>
-    <row r="22" spans="3:6">
-      <c r="C22" s="4"/>
-      <c r="D22" s="5" t="s">
+      <c r="D28" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E28" s="5">
+        <v>5</v>
+      </c>
+      <c r="F28" s="3"/>
+    </row>
+    <row r="29" spans="3:6">
+      <c r="C29" s="14"/>
+      <c r="D29" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E29" s="5">
+        <v>5</v>
+      </c>
+      <c r="F29" s="3"/>
+    </row>
+    <row r="30" spans="3:6">
+      <c r="C30" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E30" s="5">
+        <v>6</v>
+      </c>
+      <c r="F30" s="3"/>
+    </row>
+    <row r="31" spans="3:6">
+      <c r="C31" s="14"/>
+      <c r="D31" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="E22" s="5">
-        <v>2</v>
-      </c>
-      <c r="F22" s="3"/>
-    </row>
-    <row r="23" spans="3:6">
-      <c r="C23" s="4"/>
-      <c r="D23" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E23" s="5">
-        <v>4</v>
-      </c>
-      <c r="F23" s="3"/>
-    </row>
-    <row r="24" spans="3:6">
-      <c r="C24" s="4"/>
-      <c r="D24" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E24" s="5">
-        <v>4</v>
-      </c>
-      <c r="F24" s="3"/>
-    </row>
-    <row r="25" spans="3:6">
-      <c r="C25" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D25" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E25" s="5">
+      <c r="E31" s="5">
+        <v>6</v>
+      </c>
+      <c r="F31" s="3"/>
+    </row>
+    <row r="32" spans="3:6">
+      <c r="C32" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E32" s="5">
+        <v>9</v>
+      </c>
+      <c r="F32" s="3"/>
+    </row>
+    <row r="33" spans="3:6">
+      <c r="C33" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E33" s="5">
+        <v>10</v>
+      </c>
+      <c r="F33" s="3"/>
+    </row>
+    <row r="34" spans="3:6">
+      <c r="C34" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F25" s="3"/>
-    </row>
-    <row r="26" spans="3:6">
-      <c r="C26" s="4"/>
-      <c r="D26" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E26" s="5">
-        <v>5</v>
-      </c>
-      <c r="F26" s="3"/>
-    </row>
-    <row r="27" spans="3:6">
-      <c r="C27" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="E27" s="5">
-        <v>6</v>
-      </c>
-      <c r="F27" s="3"/>
-    </row>
-    <row r="28" spans="3:6">
-      <c r="C28" s="4"/>
-      <c r="D28" s="5" t="s">
+      <c r="D34" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E34" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="E28" s="5">
-        <v>6</v>
-      </c>
-      <c r="F28" s="3"/>
-    </row>
-    <row r="29" spans="3:6">
-      <c r="C29" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E29" s="5">
-        <v>9</v>
-      </c>
-      <c r="F29" s="3"/>
-    </row>
-    <row r="30" spans="3:6">
-      <c r="C30" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="E30" s="5">
-        <v>10</v>
-      </c>
-      <c r="F30" s="3"/>
-    </row>
-    <row r="31" spans="3:6">
-      <c r="C31" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E31" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="F31" s="3"/>
+      <c r="F34" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="C7:C14"/>
-    <mergeCell ref="C15:C18"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="C21:C24"/>
-    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="C7:C15"/>
+    <mergeCell ref="C16:C19"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="C22:C27"/>
+    <mergeCell ref="C28:C29"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Combat System & WeaponSystem & Player Stat
1. 컴벳 시스템
-> 몬스터가 피격되는 거 구현
-> 플레이어 피격은 구현안됨
2. 웨폰 시스템
3. 플레이어 스텟
</commit_message>
<xml_diff>
--- a/기능구현서.xlsx
+++ b/기능구현서.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
   <si>
     <t>구현 내용</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -221,11 +221,50 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>몬스터 공격과 플레이어 공격 --&gt; 컴벳 시스템 구현</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>플레이어 스탯</t>
+    <t>컴벳 시스템</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>컴벳 시스템 구현</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>웨폰 시스템 구현</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>쌤 코드 이식</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>쌤 코드 이식 후 내 게임에 맞게 리펙토링</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>공격 시에만 콜라이더 보이게 설정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>플레이어 스탯(정확히는 플레이어 싱글톤 화)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>만드려고 한건 아니지만 컴벳, 웨폰 시스템 만들면서 필요해서 만들어 버림</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>장비 수치를 플레이어 스탯에 더하면 될듯?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이건 2D 때도 했는데, 액션 리스트로 더 잘 만들어보면 돼고</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>무기 스탯 구현</t>
+  </si>
+  <si>
+    <t>공격속도는 애니메이션 재생속도를 조절해서 구현하고 싶은데 방법을 모름</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -233,7 +272,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -298,7 +337,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -321,13 +360,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -382,8 +458,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -393,8 +478,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFF8585"/>
       <color rgb="FFFFFF65"/>
-      <color rgb="FFFF8585"/>
       <color rgb="FFBEE395"/>
     </mruColors>
   </colors>
@@ -672,13 +757,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C5:J34"/>
+  <dimension ref="C5:J37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="15.875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="48.75" style="1" customWidth="1"/>
@@ -686,7 +771,7 @@
     <col min="6" max="6" width="69.125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="3:10">
+    <row r="5" spans="3:10" x14ac:dyDescent="0.3">
       <c r="H5" t="s">
         <v>35</v>
       </c>
@@ -697,7 +782,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="3:10">
+    <row r="6" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C6" s="3" t="s">
         <v>8</v>
       </c>
@@ -714,8 +799,8 @@
       <c r="I6" s="10"/>
       <c r="J6" s="11"/>
     </row>
-    <row r="7" spans="3:10">
-      <c r="C7" s="17" t="s">
+    <row r="7" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C7" s="18" t="s">
         <v>7</v>
       </c>
       <c r="D7" s="8" t="s">
@@ -726,8 +811,8 @@
       </c>
       <c r="F7" s="3"/>
     </row>
-    <row r="8" spans="3:10">
-      <c r="C8" s="17"/>
+    <row r="8" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C8" s="18"/>
       <c r="D8" s="9" t="s">
         <v>36</v>
       </c>
@@ -736,8 +821,8 @@
       </c>
       <c r="F8" s="3"/>
     </row>
-    <row r="9" spans="3:10">
-      <c r="C9" s="17"/>
+    <row r="9" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C9" s="18"/>
       <c r="D9" s="5" t="s">
         <v>6</v>
       </c>
@@ -746,8 +831,8 @@
       </c>
       <c r="F9" s="3"/>
     </row>
-    <row r="10" spans="3:10" ht="115.5">
-      <c r="C10" s="17"/>
+    <row r="10" spans="3:10" ht="115.5" x14ac:dyDescent="0.3">
+      <c r="C10" s="18"/>
       <c r="D10" s="12" t="s">
         <v>38</v>
       </c>
@@ -758,8 +843,8 @@
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="3:10">
-      <c r="C11" s="17"/>
+    <row r="11" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C11" s="18"/>
       <c r="D11" s="12" t="s">
         <v>39</v>
       </c>
@@ -768,8 +853,8 @@
       </c>
       <c r="F11" s="13"/>
     </row>
-    <row r="12" spans="3:10">
-      <c r="C12" s="17"/>
+    <row r="12" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C12" s="18"/>
       <c r="D12" s="12" t="s">
         <v>37</v>
       </c>
@@ -778,8 +863,8 @@
       </c>
       <c r="F12" s="3"/>
     </row>
-    <row r="13" spans="3:10">
-      <c r="C13" s="17"/>
+    <row r="13" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C13" s="18"/>
       <c r="D13" s="5" t="s">
         <v>40</v>
       </c>
@@ -788,8 +873,8 @@
       </c>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="3:10">
-      <c r="C14" s="17"/>
+    <row r="14" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C14" s="18"/>
       <c r="D14" s="16" t="s">
         <v>9</v>
       </c>
@@ -800,18 +885,20 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="3:10">
-      <c r="C15" s="17"/>
-      <c r="D15" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="E15" s="15">
-        <v>2</v>
-      </c>
-      <c r="F15" s="14"/>
-    </row>
-    <row r="16" spans="3:10">
-      <c r="C16" s="17"/>
+    <row r="15" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C15" s="18"/>
+      <c r="D15" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="E15" s="12">
+        <v>3</v>
+      </c>
+      <c r="F15" s="14" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C16" s="18"/>
       <c r="D16" s="7" t="s">
         <v>30</v>
       </c>
@@ -820,8 +907,8 @@
       </c>
       <c r="F16" s="3"/>
     </row>
-    <row r="17" spans="3:6">
-      <c r="C17" s="17" t="s">
+    <row r="17" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C17" s="18" t="s">
         <v>4</v>
       </c>
       <c r="D17" s="5" t="s">
@@ -832,8 +919,8 @@
       </c>
       <c r="F17" s="3"/>
     </row>
-    <row r="18" spans="3:6">
-      <c r="C18" s="17"/>
+    <row r="18" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C18" s="18"/>
       <c r="D18" s="5" t="s">
         <v>11</v>
       </c>
@@ -842,8 +929,8 @@
       </c>
       <c r="F18" s="3"/>
     </row>
-    <row r="19" spans="3:6">
-      <c r="C19" s="17"/>
+    <row r="19" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C19" s="18"/>
       <c r="D19" s="5" t="s">
         <v>12</v>
       </c>
@@ -852,8 +939,8 @@
       </c>
       <c r="F19" s="3"/>
     </row>
-    <row r="20" spans="3:6">
-      <c r="C20" s="17"/>
+    <row r="20" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C20" s="18"/>
       <c r="D20" s="5" t="s">
         <v>13</v>
       </c>
@@ -862,8 +949,8 @@
       </c>
       <c r="F20" s="3"/>
     </row>
-    <row r="21" spans="3:6">
-      <c r="C21" s="17" t="s">
+    <row r="21" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C21" s="18" t="s">
         <v>17</v>
       </c>
       <c r="D21" s="5" t="s">
@@ -872,20 +959,24 @@
       <c r="E21" s="5">
         <v>7</v>
       </c>
-      <c r="F21" s="3"/>
-    </row>
-    <row r="22" spans="3:6">
-      <c r="C22" s="17"/>
+      <c r="F21" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="22" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C22" s="18"/>
       <c r="D22" s="5" t="s">
         <v>14</v>
       </c>
       <c r="E22" s="5">
         <v>7</v>
       </c>
-      <c r="F22" s="3"/>
-    </row>
-    <row r="23" spans="3:6" ht="49.5">
-      <c r="C23" s="17" t="s">
+      <c r="F22" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="23" spans="3:6" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="C23" s="18" t="s">
         <v>21</v>
       </c>
       <c r="D23" s="12" t="s">
@@ -898,8 +989,8 @@
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="3:6" ht="82.5">
-      <c r="C24" s="17"/>
+    <row r="24" spans="3:6" ht="82.5" x14ac:dyDescent="0.3">
+      <c r="C24" s="18"/>
       <c r="D24" s="16" t="s">
         <v>43</v>
       </c>
@@ -910,124 +1001,163 @@
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="3:6">
-      <c r="C25" s="17"/>
-      <c r="D25" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="E25" s="15">
-        <v>2</v>
-      </c>
-      <c r="F25" s="4"/>
-    </row>
-    <row r="26" spans="3:6">
-      <c r="C26" s="17"/>
+    <row r="25" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C25" s="18"/>
+      <c r="D25" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E25" s="5">
+        <v>4</v>
+      </c>
+      <c r="F25" s="3"/>
+    </row>
+    <row r="26" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C26" s="18"/>
       <c r="D26" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E26" s="5">
         <v>4</v>
       </c>
       <c r="F26" s="3"/>
     </row>
-    <row r="27" spans="3:6">
-      <c r="C27" s="17"/>
-      <c r="D27" s="5" t="s">
-        <v>19</v>
+    <row r="27" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C27" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>16</v>
       </c>
       <c r="E27" s="5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F27" s="3"/>
     </row>
-    <row r="28" spans="3:6">
-      <c r="C28" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="D28" s="6" t="s">
-        <v>16</v>
+    <row r="28" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C28" s="18"/>
+      <c r="D28" s="5" t="s">
+        <v>20</v>
       </c>
       <c r="E28" s="5">
         <v>5</v>
       </c>
       <c r="F28" s="3"/>
     </row>
-    <row r="29" spans="3:6">
-      <c r="C29" s="17"/>
+    <row r="29" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C29" s="18" t="s">
+        <v>24</v>
+      </c>
       <c r="D29" s="5" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E29" s="5">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F29" s="3"/>
     </row>
-    <row r="30" spans="3:6">
-      <c r="C30" s="17" t="s">
-        <v>24</v>
-      </c>
+    <row r="30" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C30" s="18"/>
       <c r="D30" s="5" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="E30" s="5">
         <v>6</v>
       </c>
       <c r="F30" s="3"/>
     </row>
-    <row r="31" spans="3:6">
-      <c r="C31" s="17"/>
+    <row r="31" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C31" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="D31" s="5" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="E31" s="5">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F31" s="3"/>
     </row>
-    <row r="32" spans="3:6">
+    <row r="32" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C32" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E32" s="5">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F32" s="3"/>
     </row>
-    <row r="33" spans="3:6">
+    <row r="33" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C33" s="3" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E33" s="5">
-        <v>10</v>
+        <v>29</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>32</v>
       </c>
       <c r="F33" s="3"/>
     </row>
-    <row r="34" spans="3:6">
-      <c r="C34" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D34" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="E34" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="F34" s="3"/>
+    <row r="34" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C34" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="D34" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="E34" s="12">
+        <v>2</v>
+      </c>
+      <c r="F34" s="17" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="35" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C35" s="20"/>
+      <c r="D35" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="E35" s="12">
+        <v>2</v>
+      </c>
+      <c r="F35" s="17" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="36" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C36" s="20"/>
+      <c r="D36" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="E36" s="15">
+        <v>3</v>
+      </c>
+      <c r="F36" s="17" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="37" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C37" s="21"/>
+      <c r="D37" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E37" s="5">
+        <v>3</v>
+      </c>
+      <c r="F37" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="C30:C31"/>
+  <mergeCells count="7">
+    <mergeCell ref="C34:C37"/>
+    <mergeCell ref="C29:C30"/>
     <mergeCell ref="C7:C16"/>
     <mergeCell ref="C17:C20"/>
     <mergeCell ref="C21:C22"/>
-    <mergeCell ref="C23:C27"/>
-    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="C23:C26"/>
+    <mergeCell ref="C27:C28"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Collider controll & Dead animation
1. 공격 시에만 콜라이더가 켜짐
2. 사망 애니메이션 적용
</commit_message>
<xml_diff>
--- a/기능구현서.xlsx
+++ b/기능구현서.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
   <si>
     <t>구현 내용</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -267,6 +267,25 @@
     <t>이슈 1) 공격속도는 애니메이션 재생속도를 조절해서 구현하고 싶은데 방법을 모름
 해결) StateMachineBehaviour를 이용해서 애니메이터의 속도 자체를 
 바꿨다가 원래대로 돌림</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>지피티는 신이야</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>몬스터 사망 애니메이션 구현</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>리펙토링</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이슈 1) 네비 매시가 꺼지지 않아 죽고나서도 이상하게 움직임
+- 리지드바디의 그래비티랑 프리즈 포지션 x, y, z를 체크함
+이슈 2) 네비 매시를 껐는데도 죽고나서 움직임
+- 리지드바디의 벨로시티가 문제. 죽을 때 0으로 초기화</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -274,7 +293,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -405,7 +424,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -468,6 +487,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -478,8 +500,8 @@
   <colors>
     <mruColors>
       <color rgb="FFBEE395"/>
+      <color rgb="FFFFFF65"/>
       <color rgb="FFFF8585"/>
-      <color rgb="FFFFFF65"/>
     </mruColors>
   </colors>
   <extLst>
@@ -756,13 +778,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C5:J37"/>
+  <dimension ref="C5:J40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36:E36"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38:E38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
     <col min="3" max="3" width="15.875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="48.75" style="1" customWidth="1"/>
@@ -770,7 +792,7 @@
     <col min="6" max="6" width="69.125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:10">
       <c r="H5" t="s">
         <v>35</v>
       </c>
@@ -781,7 +803,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:10">
       <c r="C6" s="3" t="s">
         <v>8</v>
       </c>
@@ -798,7 +820,7 @@
       <c r="I6" s="10"/>
       <c r="J6" s="11"/>
     </row>
-    <row r="7" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="3:10">
       <c r="C7" s="20" t="s">
         <v>7</v>
       </c>
@@ -810,7 +832,7 @@
       </c>
       <c r="F7" s="3"/>
     </row>
-    <row r="8" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="3:10">
       <c r="C8" s="20"/>
       <c r="D8" s="9" t="s">
         <v>36</v>
@@ -820,7 +842,7 @@
       </c>
       <c r="F8" s="3"/>
     </row>
-    <row r="9" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="3:10">
       <c r="C9" s="20"/>
       <c r="D9" s="5" t="s">
         <v>6</v>
@@ -830,7 +852,7 @@
       </c>
       <c r="F9" s="3"/>
     </row>
-    <row r="10" spans="3:10" ht="115.5" x14ac:dyDescent="0.3">
+    <row r="10" spans="3:10" ht="115.5">
       <c r="C10" s="20"/>
       <c r="D10" s="12" t="s">
         <v>38</v>
@@ -842,7 +864,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="3:10">
       <c r="C11" s="20"/>
       <c r="D11" s="12" t="s">
         <v>39</v>
@@ -852,7 +874,7 @@
       </c>
       <c r="F11" s="13"/>
     </row>
-    <row r="12" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="3:10">
       <c r="C12" s="20"/>
       <c r="D12" s="12" t="s">
         <v>37</v>
@@ -862,7 +884,7 @@
       </c>
       <c r="F12" s="3"/>
     </row>
-    <row r="13" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="3:10">
       <c r="C13" s="20"/>
       <c r="D13" s="5" t="s">
         <v>40</v>
@@ -872,7 +894,7 @@
       </c>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="3:10">
       <c r="C14" s="20"/>
       <c r="D14" s="15" t="s">
         <v>9</v>
@@ -884,7 +906,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="3:10">
       <c r="C15" s="20"/>
       <c r="D15" s="15" t="s">
         <v>53</v>
@@ -896,7 +918,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="16" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="3:10">
       <c r="C16" s="20"/>
       <c r="D16" s="7" t="s">
         <v>30</v>
@@ -906,7 +928,7 @@
       </c>
       <c r="F16" s="3"/>
     </row>
-    <row r="17" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:6">
       <c r="C17" s="20" t="s">
         <v>4</v>
       </c>
@@ -918,7 +940,7 @@
       </c>
       <c r="F17" s="3"/>
     </row>
-    <row r="18" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:6">
       <c r="C18" s="20"/>
       <c r="D18" s="5" t="s">
         <v>11</v>
@@ -928,7 +950,7 @@
       </c>
       <c r="F18" s="3"/>
     </row>
-    <row r="19" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:6">
       <c r="C19" s="20"/>
       <c r="D19" s="5" t="s">
         <v>12</v>
@@ -938,7 +960,7 @@
       </c>
       <c r="F19" s="3"/>
     </row>
-    <row r="20" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:6">
       <c r="C20" s="20"/>
       <c r="D20" s="5" t="s">
         <v>13</v>
@@ -948,7 +970,7 @@
       </c>
       <c r="F20" s="3"/>
     </row>
-    <row r="21" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:6">
       <c r="C21" s="20" t="s">
         <v>17</v>
       </c>
@@ -962,7 +984,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="22" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:6">
       <c r="C22" s="20"/>
       <c r="D22" s="5" t="s">
         <v>14</v>
@@ -974,7 +996,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="23" spans="3:6" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="23" spans="3:6" ht="49.5">
       <c r="C23" s="20" t="s">
         <v>21</v>
       </c>
@@ -988,7 +1010,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="3:6" ht="82.5" x14ac:dyDescent="0.3">
+    <row r="24" spans="3:6" ht="82.5">
       <c r="C24" s="20"/>
       <c r="D24" s="15" t="s">
         <v>43</v>
@@ -1000,7 +1022,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="3:6">
       <c r="C25" s="20"/>
       <c r="D25" s="5" t="s">
         <v>18</v>
@@ -1010,153 +1032,173 @@
       </c>
       <c r="F25" s="3"/>
     </row>
-    <row r="26" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="3:6" ht="66">
       <c r="C26" s="20"/>
-      <c r="D26" s="5" t="s">
+      <c r="D26" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="E26" s="12">
+        <v>3</v>
+      </c>
+      <c r="F26" s="13" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="27" spans="3:6">
+      <c r="C27" s="20"/>
+      <c r="D27" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E26" s="5">
+      <c r="E27" s="5">
         <v>4</v>
       </c>
-      <c r="F26" s="3"/>
-    </row>
-    <row r="27" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C27" s="20" t="s">
+      <c r="F27" s="3"/>
+    </row>
+    <row r="28" spans="3:6">
+      <c r="C28" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="D27" s="6" t="s">
+      <c r="D28" s="6" t="s">
         <v>16</v>
-      </c>
-      <c r="E27" s="5">
-        <v>5</v>
-      </c>
-      <c r="F27" s="3"/>
-    </row>
-    <row r="28" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C28" s="20"/>
-      <c r="D28" s="5" t="s">
-        <v>20</v>
       </c>
       <c r="E28" s="5">
         <v>5</v>
       </c>
       <c r="F28" s="3"/>
     </row>
-    <row r="29" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C29" s="20" t="s">
+    <row r="29" spans="3:6">
+      <c r="C29" s="20"/>
+      <c r="D29" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E29" s="5">
+        <v>5</v>
+      </c>
+      <c r="F29" s="3"/>
+    </row>
+    <row r="30" spans="3:6">
+      <c r="C30" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="D29" s="5" t="s">
+      <c r="D30" s="5" t="s">
         <v>23</v>
-      </c>
-      <c r="E29" s="5">
-        <v>6</v>
-      </c>
-      <c r="F29" s="3"/>
-    </row>
-    <row r="30" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C30" s="20"/>
-      <c r="D30" s="5" t="s">
-        <v>31</v>
       </c>
       <c r="E30" s="5">
         <v>6</v>
       </c>
       <c r="F30" s="3"/>
     </row>
-    <row r="31" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C31" s="3" t="s">
+    <row r="31" spans="3:6">
+      <c r="C31" s="20"/>
+      <c r="D31" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E31" s="5">
+        <v>6</v>
+      </c>
+      <c r="F31" s="3"/>
+    </row>
+    <row r="32" spans="3:6">
+      <c r="C32" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D31" s="5" t="s">
+      <c r="D32" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="E31" s="5">
+      <c r="E32" s="5">
         <v>9</v>
       </c>
-      <c r="F31" s="3"/>
-    </row>
-    <row r="32" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C32" s="3" t="s">
+      <c r="F32" s="3"/>
+    </row>
+    <row r="33" spans="3:6">
+      <c r="C33" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D32" s="5" t="s">
+      <c r="D33" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E32" s="5">
+      <c r="E33" s="5">
         <v>10</v>
       </c>
-      <c r="F32" s="3"/>
-    </row>
-    <row r="33" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C33" s="3" t="s">
+      <c r="F33" s="3"/>
+    </row>
+    <row r="34" spans="3:6">
+      <c r="C34" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D33" s="5" t="s">
+      <c r="D34" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="E33" s="5" t="s">
+      <c r="E34" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="F33" s="3"/>
-    </row>
-    <row r="34" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C34" s="17" t="s">
+      <c r="F34" s="3"/>
+    </row>
+    <row r="35" spans="3:6">
+      <c r="C35" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="D34" s="12" t="s">
+      <c r="D35" s="12" t="s">
         <v>48</v>
-      </c>
-      <c r="E34" s="12">
-        <v>2</v>
-      </c>
-      <c r="F34" s="16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="35" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C35" s="18"/>
-      <c r="D35" s="12" t="s">
-        <v>49</v>
       </c>
       <c r="E35" s="12">
         <v>2</v>
       </c>
       <c r="F35" s="16" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="36" spans="3:6" ht="66" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="36" spans="3:6">
       <c r="C36" s="18"/>
       <c r="D36" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="E36" s="12">
+        <v>2</v>
+      </c>
+      <c r="F36" s="16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="37" spans="3:6" ht="66">
+      <c r="C37" s="18"/>
+      <c r="D37" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="E36" s="12">
+      <c r="E37" s="12">
         <v>3</v>
       </c>
-      <c r="F36" s="13" t="s">
+      <c r="F37" s="13" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="37" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C37" s="19"/>
-      <c r="D37" s="5" t="s">
+    <row r="38" spans="3:6">
+      <c r="C38" s="19"/>
+      <c r="D38" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="E37" s="5">
+      <c r="E38" s="12">
         <v>3</v>
       </c>
-      <c r="F37" s="16"/>
+      <c r="F38" s="16" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="40" spans="3:6">
+      <c r="C40" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D40" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="C34:C37"/>
-    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="C35:C38"/>
+    <mergeCell ref="C30:C31"/>
     <mergeCell ref="C7:C16"/>
     <mergeCell ref="C17:C20"/>
     <mergeCell ref="C21:C22"/>
-    <mergeCell ref="C23:C26"/>
-    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="C23:C27"/>
+    <mergeCell ref="C28:C29"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Link (Skill System & UI System & Gem System)
UI를 통해 젬 데이터를 관리하고 스킬에 까지 변동이 생기도록 세 시스템을 연동
</commit_message>
<xml_diff>
--- a/기능구현서.xlsx
+++ b/기능구현서.xlsx
@@ -463,7 +463,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -516,9 +516,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -541,8 +538,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFBEE395"/>
       <color rgb="FFFFFF65"/>
-      <color rgb="FFBEE395"/>
       <color rgb="FFFF8585"/>
     </mruColors>
   </colors>
@@ -822,8 +819,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C5:J43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B11" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" topLeftCell="B5" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -863,7 +860,7 @@
       <c r="J6" s="10"/>
     </row>
     <row r="7" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C7" s="22" t="s">
+      <c r="C7" s="21" t="s">
         <v>7</v>
       </c>
       <c r="D7" s="7" t="s">
@@ -875,7 +872,7 @@
       <c r="F7" s="3"/>
     </row>
     <row r="8" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C8" s="22"/>
+      <c r="C8" s="21"/>
       <c r="D8" s="8" t="s">
         <v>35</v>
       </c>
@@ -885,7 +882,7 @@
       <c r="F8" s="3"/>
     </row>
     <row r="9" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C9" s="22"/>
+      <c r="C9" s="21"/>
       <c r="D9" s="5" t="s">
         <v>6</v>
       </c>
@@ -895,7 +892,7 @@
       <c r="F9" s="3"/>
     </row>
     <row r="10" spans="3:10" ht="99" x14ac:dyDescent="0.3">
-      <c r="C10" s="22"/>
+      <c r="C10" s="21"/>
       <c r="D10" s="11" t="s">
         <v>37</v>
       </c>
@@ -907,7 +904,7 @@
       </c>
     </row>
     <row r="11" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C11" s="22"/>
+      <c r="C11" s="21"/>
       <c r="D11" s="11" t="s">
         <v>38</v>
       </c>
@@ -917,7 +914,7 @@
       <c r="F11" s="12"/>
     </row>
     <row r="12" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C12" s="22"/>
+      <c r="C12" s="21"/>
       <c r="D12" s="11" t="s">
         <v>36</v>
       </c>
@@ -927,7 +924,7 @@
       <c r="F12" s="3"/>
     </row>
     <row r="13" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C13" s="22"/>
+      <c r="C13" s="21"/>
       <c r="D13" s="5" t="s">
         <v>39</v>
       </c>
@@ -937,7 +934,7 @@
       <c r="F13" s="4"/>
     </row>
     <row r="14" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C14" s="22"/>
+      <c r="C14" s="21"/>
       <c r="D14" s="14" t="s">
         <v>9</v>
       </c>
@@ -949,7 +946,7 @@
       </c>
     </row>
     <row r="15" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C15" s="22"/>
+      <c r="C15" s="21"/>
       <c r="D15" s="14" t="s">
         <v>50</v>
       </c>
@@ -961,7 +958,7 @@
       </c>
     </row>
     <row r="16" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C16" s="22"/>
+      <c r="C16" s="21"/>
       <c r="D16" s="6" t="s">
         <v>29</v>
       </c>
@@ -971,13 +968,13 @@
       <c r="F16" s="3"/>
     </row>
     <row r="17" spans="3:6" ht="198" x14ac:dyDescent="0.3">
-      <c r="C17" s="22" t="s">
+      <c r="C17" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="D17" s="18" t="s">
+      <c r="D17" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="E17" s="18">
+      <c r="E17" s="11">
         <v>4</v>
       </c>
       <c r="F17" s="12" t="s">
@@ -985,7 +982,7 @@
       </c>
     </row>
     <row r="18" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C18" s="22"/>
+      <c r="C18" s="21"/>
       <c r="D18" s="5" t="s">
         <v>11</v>
       </c>
@@ -995,7 +992,7 @@
       <c r="F18" s="3"/>
     </row>
     <row r="19" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C19" s="22"/>
+      <c r="C19" s="21"/>
       <c r="D19" s="11" t="s">
         <v>61</v>
       </c>
@@ -1007,7 +1004,7 @@
       </c>
     </row>
     <row r="20" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C20" s="22"/>
+      <c r="C20" s="21"/>
       <c r="D20" s="11" t="s">
         <v>12</v>
       </c>
@@ -1017,11 +1014,11 @@
       <c r="F20" s="17"/>
     </row>
     <row r="21" spans="3:6" ht="66" x14ac:dyDescent="0.3">
-      <c r="C21" s="22"/>
-      <c r="D21" s="18" t="s">
+      <c r="C21" s="21"/>
+      <c r="D21" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="E21" s="18">
+      <c r="E21" s="11">
         <v>4</v>
       </c>
       <c r="F21" s="12" t="s">
@@ -1029,7 +1026,7 @@
       </c>
     </row>
     <row r="22" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C22" s="22" t="s">
+      <c r="C22" s="21" t="s">
         <v>16</v>
       </c>
       <c r="D22" s="5" t="s">
@@ -1043,7 +1040,7 @@
       </c>
     </row>
     <row r="23" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C23" s="22"/>
+      <c r="C23" s="21"/>
       <c r="D23" s="5" t="s">
         <v>13</v>
       </c>
@@ -1055,7 +1052,7 @@
       </c>
     </row>
     <row r="24" spans="3:6" ht="33" x14ac:dyDescent="0.3">
-      <c r="C24" s="22" t="s">
+      <c r="C24" s="21" t="s">
         <v>20</v>
       </c>
       <c r="D24" s="11" t="s">
@@ -1069,7 +1066,7 @@
       </c>
     </row>
     <row r="25" spans="3:6" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="C25" s="22"/>
+      <c r="C25" s="21"/>
       <c r="D25" s="14" t="s">
         <v>42</v>
       </c>
@@ -1081,7 +1078,7 @@
       </c>
     </row>
     <row r="26" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C26" s="22"/>
+      <c r="C26" s="21"/>
       <c r="D26" s="5" t="s">
         <v>17</v>
       </c>
@@ -1091,7 +1088,7 @@
       <c r="F26" s="3"/>
     </row>
     <row r="27" spans="3:6" ht="82.5" x14ac:dyDescent="0.3">
-      <c r="C27" s="22"/>
+      <c r="C27" s="21"/>
       <c r="D27" s="11" t="s">
         <v>55</v>
       </c>
@@ -1103,7 +1100,7 @@
       </c>
     </row>
     <row r="28" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C28" s="22"/>
+      <c r="C28" s="21"/>
       <c r="D28" s="5" t="s">
         <v>57</v>
       </c>
@@ -1113,7 +1110,7 @@
       <c r="F28" s="12"/>
     </row>
     <row r="29" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C29" s="22"/>
+      <c r="C29" s="21"/>
       <c r="D29" s="5" t="s">
         <v>62</v>
       </c>
@@ -1123,7 +1120,7 @@
       <c r="F29" s="12"/>
     </row>
     <row r="30" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C30" s="22"/>
+      <c r="C30" s="21"/>
       <c r="D30" s="5" t="s">
         <v>18</v>
       </c>
@@ -1133,7 +1130,7 @@
       <c r="F30" s="3"/>
     </row>
     <row r="31" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C31" s="22" t="s">
+      <c r="C31" s="21" t="s">
         <v>21</v>
       </c>
       <c r="D31" s="14" t="s">
@@ -1145,7 +1142,7 @@
       <c r="F31" s="3"/>
     </row>
     <row r="32" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C32" s="22"/>
+      <c r="C32" s="21"/>
       <c r="D32" s="5" t="s">
         <v>19</v>
       </c>
@@ -1155,7 +1152,7 @@
       <c r="F32" s="3"/>
     </row>
     <row r="33" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C33" s="22" t="s">
+      <c r="C33" s="21" t="s">
         <v>23</v>
       </c>
       <c r="D33" s="5" t="s">
@@ -1167,7 +1164,7 @@
       <c r="F33" s="3"/>
     </row>
     <row r="34" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C34" s="22"/>
+      <c r="C34" s="21"/>
       <c r="D34" s="5" t="s">
         <v>30</v>
       </c>
@@ -1213,7 +1210,7 @@
       <c r="F37" s="3"/>
     </row>
     <row r="38" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C38" s="19" t="s">
+      <c r="C38" s="18" t="s">
         <v>44</v>
       </c>
       <c r="D38" s="11" t="s">
@@ -1227,7 +1224,7 @@
       </c>
     </row>
     <row r="39" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C39" s="20"/>
+      <c r="C39" s="19"/>
       <c r="D39" s="11" t="s">
         <v>46</v>
       </c>
@@ -1239,7 +1236,7 @@
       </c>
     </row>
     <row r="40" spans="3:6" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="C40" s="20"/>
+      <c r="C40" s="19"/>
       <c r="D40" s="11" t="s">
         <v>53</v>
       </c>
@@ -1251,7 +1248,7 @@
       </c>
     </row>
     <row r="41" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C41" s="21"/>
+      <c r="C41" s="20"/>
       <c r="D41" s="11" t="s">
         <v>49</v>
       </c>

</xml_diff>

<commit_message>
Make FireBallGem & Skill
1. FireBallGem은 프로토타입 과정에서 이미 만듬

2. Fire ball skill을 구현
(근데, 컴벳 시스템이랑 연동도 안했고 때문에 데미지 연산이 필요 없어서 플레이어 스텟이랑도 연동 안함 나중에 할 것)
</commit_message>
<xml_diff>
--- a/기능구현서.xlsx
+++ b/기능구현서.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
   <si>
     <t>구현 내용</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -325,6 +325,10 @@
 해결) 얼추 주먹구구식으로 만들었는데 구조가 매우 끔찍함
 이슈 2) 구조가 매우 끔찍함. 리펙토링 해야함
 해결) 스킬 젬 시스템을 따로 구성하고 구조화 함</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>시스템들을 구조화 해놓으니까 스킬 젬 만드는건 3분만에 바로 됌</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -819,8 +823,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C5:J43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B5" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -983,13 +987,15 @@
     </row>
     <row r="18" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C18" s="21"/>
-      <c r="D18" s="5" t="s">
+      <c r="D18" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E18" s="5">
+      <c r="E18" s="11">
         <v>4</v>
       </c>
-      <c r="F18" s="3"/>
+      <c r="F18" s="3" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="19" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C19" s="21"/>

</xml_diff>

<commit_message>
Skill Animation & Skill Damage Setting
1. 스킬 시전 모션과 시전 위치, 애니메이션 완료

2. 스킬 데미지 설정. 컴벳시스템과 연동
</commit_message>
<xml_diff>
--- a/기능구현서.xlsx
+++ b/기능구현서.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="73">
   <si>
     <t>구현 내용</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -328,7 +328,16 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>시스템들을 구조화 해놓으니까 스킬 젬 만드는건 3분만에 바로 됌</t>
+    <t>스킬 시전 애니메이션</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>나중에 스킬 태그(e,g., 투사체인지, 즉발인지)를 통해 다른 애니메이션 나오도록</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>시스템들을 구조화 해놓으니까 스킬 젬 만드는건 3분만에 바로 됌
+구조화는 신이야! 데미지 처리도 복붙으로 끝나네</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -821,10 +830,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C5:J43"/>
+  <dimension ref="C5:J44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="B10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -972,7 +981,7 @@
       <c r="F16" s="3"/>
     </row>
     <row r="17" spans="3:6" ht="198" x14ac:dyDescent="0.3">
-      <c r="C17" s="21" t="s">
+      <c r="C17" s="18" t="s">
         <v>4</v>
       </c>
       <c r="D17" s="11" t="s">
@@ -985,20 +994,20 @@
         <v>66</v>
       </c>
     </row>
-    <row r="18" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C18" s="21"/>
+    <row r="18" spans="3:6" ht="33" x14ac:dyDescent="0.3">
+      <c r="C18" s="19"/>
       <c r="D18" s="11" t="s">
         <v>11</v>
       </c>
       <c r="E18" s="11">
         <v>4</v>
       </c>
-      <c r="F18" s="3" t="s">
-        <v>70</v>
+      <c r="F18" s="12" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="19" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C19" s="21"/>
+      <c r="C19" s="19"/>
       <c r="D19" s="11" t="s">
         <v>61</v>
       </c>
@@ -1010,7 +1019,7 @@
       </c>
     </row>
     <row r="20" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C20" s="21"/>
+      <c r="C20" s="19"/>
       <c r="D20" s="11" t="s">
         <v>12</v>
       </c>
@@ -1020,7 +1029,7 @@
       <c r="F20" s="17"/>
     </row>
     <row r="21" spans="3:6" ht="66" x14ac:dyDescent="0.3">
-      <c r="C21" s="21"/>
+      <c r="C21" s="19"/>
       <c r="D21" s="11" t="s">
         <v>68</v>
       </c>
@@ -1032,93 +1041,95 @@
       </c>
     </row>
     <row r="22" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C22" s="21" t="s">
+      <c r="C22" s="20"/>
+      <c r="D22" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="E22" s="11">
+        <v>4</v>
+      </c>
+      <c r="F22" s="12" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="23" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C23" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="D23" s="5" t="s">
         <v>14</v>
-      </c>
-      <c r="E22" s="5">
-        <v>7</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="23" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C23" s="21"/>
-      <c r="D23" s="5" t="s">
-        <v>13</v>
       </c>
       <c r="E23" s="5">
         <v>7</v>
       </c>
       <c r="F23" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="24" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C24" s="21"/>
+      <c r="D24" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E24" s="5">
+        <v>7</v>
+      </c>
+      <c r="F24" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="24" spans="3:6" ht="33" x14ac:dyDescent="0.3">
-      <c r="C24" s="21" t="s">
+    <row r="25" spans="3:6" ht="33" x14ac:dyDescent="0.3">
+      <c r="C25" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="D24" s="11" t="s">
+      <c r="D25" s="11" t="s">
         <v>41</v>
-      </c>
-      <c r="E24" s="11">
-        <v>2</v>
-      </c>
-      <c r="F24" s="12" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="25" spans="3:6" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="C25" s="21"/>
-      <c r="D25" s="14" t="s">
-        <v>42</v>
       </c>
       <c r="E25" s="11">
         <v>2</v>
       </c>
       <c r="F25" s="12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="26" spans="3:6" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="C26" s="21"/>
+      <c r="D26" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="E26" s="11">
+        <v>2</v>
+      </c>
+      <c r="F26" s="12" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="26" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C26" s="21"/>
-      <c r="D26" s="5" t="s">
+    <row r="27" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C27" s="21"/>
+      <c r="D27" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E26" s="5">
+      <c r="E27" s="5">
         <v>5</v>
       </c>
-      <c r="F26" s="3"/>
-    </row>
-    <row r="27" spans="3:6" ht="82.5" x14ac:dyDescent="0.3">
-      <c r="C27" s="21"/>
-      <c r="D27" s="11" t="s">
+      <c r="F27" s="3"/>
+    </row>
+    <row r="28" spans="3:6" ht="82.5" x14ac:dyDescent="0.3">
+      <c r="C28" s="21"/>
+      <c r="D28" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="E27" s="11">
+      <c r="E28" s="11">
         <v>3</v>
       </c>
-      <c r="F27" s="12" t="s">
+      <c r="F28" s="12" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="28" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C28" s="21"/>
-      <c r="D28" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="E28" s="5">
-        <v>5</v>
-      </c>
-      <c r="F28" s="12"/>
     </row>
     <row r="29" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C29" s="21"/>
       <c r="D29" s="5" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="E29" s="5">
         <v>5</v>
@@ -1128,51 +1139,51 @@
     <row r="30" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C30" s="21"/>
       <c r="D30" s="5" t="s">
-        <v>18</v>
+        <v>62</v>
       </c>
       <c r="E30" s="5">
         <v>5</v>
       </c>
-      <c r="F30" s="3"/>
+      <c r="F30" s="12"/>
     </row>
     <row r="31" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C31" s="21" t="s">
+      <c r="C31" s="21"/>
+      <c r="D31" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E31" s="5">
+        <v>5</v>
+      </c>
+      <c r="F31" s="3"/>
+    </row>
+    <row r="32" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C32" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="D31" s="14" t="s">
+      <c r="D32" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="E31" s="11">
+      <c r="E32" s="11">
         <v>4</v>
       </c>
-      <c r="F31" s="3"/>
-    </row>
-    <row r="32" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C32" s="21"/>
-      <c r="D32" s="5" t="s">
+      <c r="F32" s="3"/>
+    </row>
+    <row r="33" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C33" s="21"/>
+      <c r="D33" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E32" s="5">
+      <c r="E33" s="5">
         <v>5</v>
       </c>
-      <c r="F32" s="3"/>
-    </row>
-    <row r="33" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C33" s="21" t="s">
+      <c r="F33" s="3"/>
+    </row>
+    <row r="34" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C34" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="D33" s="5" t="s">
+      <c r="D34" s="5" t="s">
         <v>22</v>
-      </c>
-      <c r="E33" s="5">
-        <v>6</v>
-      </c>
-      <c r="F33" s="3"/>
-    </row>
-    <row r="34" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C34" s="21"/>
-      <c r="D34" s="5" t="s">
-        <v>30</v>
       </c>
       <c r="E34" s="5">
         <v>6</v>
@@ -1180,106 +1191,116 @@
       <c r="F34" s="3"/>
     </row>
     <row r="35" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C35" s="3" t="s">
-        <v>24</v>
-      </c>
+      <c r="C35" s="21"/>
       <c r="D35" s="5" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="E35" s="5">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F35" s="3"/>
     </row>
     <row r="36" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C36" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E36" s="5">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F36" s="3"/>
     </row>
     <row r="37" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C37" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E37" s="5">
+        <v>10</v>
+      </c>
+      <c r="F37" s="3"/>
+    </row>
+    <row r="38" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C38" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D37" s="5" t="s">
+      <c r="D38" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E37" s="5" t="s">
+      <c r="E38" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="F37" s="3"/>
-    </row>
-    <row r="38" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C38" s="18" t="s">
+      <c r="F38" s="3"/>
+    </row>
+    <row r="39" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C39" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="D38" s="11" t="s">
+      <c r="D39" s="11" t="s">
         <v>45</v>
-      </c>
-      <c r="E38" s="11">
-        <v>2</v>
-      </c>
-      <c r="F38" s="15" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="39" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C39" s="19"/>
-      <c r="D39" s="11" t="s">
-        <v>46</v>
       </c>
       <c r="E39" s="11">
         <v>2</v>
       </c>
       <c r="F39" s="15" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="40" spans="3:6" ht="49.5" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="40" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C40" s="19"/>
       <c r="D40" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="E40" s="11">
+        <v>2</v>
+      </c>
+      <c r="F40" s="15" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="41" spans="3:6" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="C41" s="19"/>
+      <c r="D41" s="11" t="s">
         <v>53</v>
-      </c>
-      <c r="E40" s="11">
-        <v>3</v>
-      </c>
-      <c r="F40" s="12" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="41" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C41" s="20"/>
-      <c r="D41" s="11" t="s">
-        <v>49</v>
       </c>
       <c r="E41" s="11">
         <v>3</v>
       </c>
-      <c r="F41" s="15" t="s">
+      <c r="F41" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="42" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C42" s="20"/>
+      <c r="D42" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="E42" s="11">
+        <v>3</v>
+      </c>
+      <c r="F42" s="15" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="43" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C43" s="1" t="s">
+    <row r="44" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C44" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D43" s="16"/>
+      <c r="D44" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="C38:C41"/>
-    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="C39:C42"/>
+    <mergeCell ref="C34:C35"/>
     <mergeCell ref="C7:C16"/>
-    <mergeCell ref="C17:C21"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="C24:C30"/>
-    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="C25:C31"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="C17:C22"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Player UI & Player Attacked
1. 플레이어 UI 제작 및 스탯과 연동
2. 플레이어가 피격을 당할 수 있게 함
</commit_message>
<xml_diff>
--- a/기능구현서.xlsx
+++ b/기능구현서.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="77">
   <si>
     <t>구현 내용</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -338,6 +338,22 @@
   <si>
     <t>시스템들을 구조화 해놓으니까 스킬 젬 만드는건 3분만에 바로 됌
 구조화는 신이야! 데미지 처리도 복붙으로 끝나네</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>스킬 사용하면 자원이 깎이게 만들기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>체력, 마나, 레벨 등의 UI 만들기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>플레이어 피격</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>플레이어 스탯과 UI 연동</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -476,7 +492,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -527,6 +543,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -830,10 +849,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C5:J44"/>
+  <dimension ref="C5:J48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -873,7 +892,7 @@
       <c r="J6" s="10"/>
     </row>
     <row r="7" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C7" s="21" t="s">
+      <c r="C7" s="22" t="s">
         <v>7</v>
       </c>
       <c r="D7" s="7" t="s">
@@ -885,7 +904,7 @@
       <c r="F7" s="3"/>
     </row>
     <row r="8" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C8" s="21"/>
+      <c r="C8" s="22"/>
       <c r="D8" s="8" t="s">
         <v>35</v>
       </c>
@@ -895,7 +914,7 @@
       <c r="F8" s="3"/>
     </row>
     <row r="9" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C9" s="21"/>
+      <c r="C9" s="22"/>
       <c r="D9" s="5" t="s">
         <v>6</v>
       </c>
@@ -905,7 +924,7 @@
       <c r="F9" s="3"/>
     </row>
     <row r="10" spans="3:10" ht="99" x14ac:dyDescent="0.3">
-      <c r="C10" s="21"/>
+      <c r="C10" s="22"/>
       <c r="D10" s="11" t="s">
         <v>37</v>
       </c>
@@ -917,7 +936,7 @@
       </c>
     </row>
     <row r="11" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C11" s="21"/>
+      <c r="C11" s="22"/>
       <c r="D11" s="11" t="s">
         <v>38</v>
       </c>
@@ -927,7 +946,7 @@
       <c r="F11" s="12"/>
     </row>
     <row r="12" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C12" s="21"/>
+      <c r="C12" s="22"/>
       <c r="D12" s="11" t="s">
         <v>36</v>
       </c>
@@ -937,7 +956,7 @@
       <c r="F12" s="3"/>
     </row>
     <row r="13" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C13" s="21"/>
+      <c r="C13" s="22"/>
       <c r="D13" s="5" t="s">
         <v>39</v>
       </c>
@@ -947,7 +966,7 @@
       <c r="F13" s="4"/>
     </row>
     <row r="14" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C14" s="21"/>
+      <c r="C14" s="22"/>
       <c r="D14" s="14" t="s">
         <v>9</v>
       </c>
@@ -959,7 +978,7 @@
       </c>
     </row>
     <row r="15" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C15" s="21"/>
+      <c r="C15" s="22"/>
       <c r="D15" s="14" t="s">
         <v>50</v>
       </c>
@@ -971,229 +990,225 @@
       </c>
     </row>
     <row r="16" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C16" s="21"/>
-      <c r="D16" s="6" t="s">
+      <c r="C16" s="22"/>
+      <c r="D16" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="E16" s="11">
+        <v>5</v>
+      </c>
+      <c r="F16" s="18"/>
+    </row>
+    <row r="17" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C17" s="22"/>
+      <c r="D17" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="E17" s="11">
+        <v>5</v>
+      </c>
+      <c r="F17" s="18"/>
+    </row>
+    <row r="18" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C18" s="22"/>
+      <c r="D18" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="E18" s="11">
+        <v>5</v>
+      </c>
+      <c r="F18" s="18"/>
+    </row>
+    <row r="19" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C19" s="22"/>
+      <c r="D19" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="E16" s="5">
+      <c r="E19" s="5">
         <v>8</v>
       </c>
-      <c r="F16" s="3"/>
-    </row>
-    <row r="17" spans="3:6" ht="198" x14ac:dyDescent="0.3">
-      <c r="C17" s="18" t="s">
+      <c r="F19" s="3"/>
+    </row>
+    <row r="20" spans="3:6" ht="198" x14ac:dyDescent="0.3">
+      <c r="C20" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="D17" s="11" t="s">
+      <c r="D20" s="11" t="s">
         <v>10</v>
-      </c>
-      <c r="E17" s="11">
-        <v>4</v>
-      </c>
-      <c r="F17" s="12" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="18" spans="3:6" ht="33" x14ac:dyDescent="0.3">
-      <c r="C18" s="19"/>
-      <c r="D18" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E18" s="11">
-        <v>4</v>
-      </c>
-      <c r="F18" s="12" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="19" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C19" s="19"/>
-      <c r="D19" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="E19" s="11">
-        <v>4</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="20" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C20" s="19"/>
-      <c r="D20" s="11" t="s">
-        <v>12</v>
       </c>
       <c r="E20" s="11">
         <v>4</v>
       </c>
-      <c r="F20" s="17"/>
-    </row>
-    <row r="21" spans="3:6" ht="66" x14ac:dyDescent="0.3">
-      <c r="C21" s="19"/>
+      <c r="F20" s="12" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="21" spans="3:6" ht="33" x14ac:dyDescent="0.3">
+      <c r="C21" s="20"/>
       <c r="D21" s="11" t="s">
-        <v>68</v>
+        <v>11</v>
       </c>
       <c r="E21" s="11">
         <v>4</v>
       </c>
       <c r="F21" s="12" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row r="22" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C22" s="20"/>
       <c r="D22" s="11" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="E22" s="11">
         <v>4</v>
       </c>
-      <c r="F22" s="12" t="s">
+      <c r="F22" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="23" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C23" s="20"/>
+      <c r="D23" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E23" s="11">
+        <v>4</v>
+      </c>
+      <c r="F23" s="17"/>
+    </row>
+    <row r="24" spans="3:6" ht="66" x14ac:dyDescent="0.3">
+      <c r="C24" s="20"/>
+      <c r="D24" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="E24" s="11">
+        <v>4</v>
+      </c>
+      <c r="F24" s="12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="25" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C25" s="20"/>
+      <c r="D25" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="E25" s="5">
+        <v>5</v>
+      </c>
+      <c r="F25" s="12"/>
+    </row>
+    <row r="26" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C26" s="21"/>
+      <c r="D26" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="E26" s="11">
+        <v>4</v>
+      </c>
+      <c r="F26" s="12" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="23" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C23" s="21" t="s">
+    <row r="27" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C27" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="D27" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E23" s="5">
+      <c r="E27" s="5">
         <v>7</v>
       </c>
-      <c r="F23" s="3" t="s">
+      <c r="F27" s="3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="24" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C24" s="21"/>
-      <c r="D24" s="5" t="s">
+    <row r="28" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C28" s="22"/>
+      <c r="D28" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E24" s="5">
+      <c r="E28" s="5">
         <v>7</v>
       </c>
-      <c r="F24" s="3" t="s">
+      <c r="F28" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="25" spans="3:6" ht="33" x14ac:dyDescent="0.3">
-      <c r="C25" s="21" t="s">
+    <row r="29" spans="3:6" ht="33" x14ac:dyDescent="0.3">
+      <c r="C29" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="D25" s="11" t="s">
+      <c r="D29" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="E25" s="11">
+      <c r="E29" s="11">
         <v>2</v>
       </c>
-      <c r="F25" s="12" t="s">
+      <c r="F29" s="12" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="26" spans="3:6" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="C26" s="21"/>
-      <c r="D26" s="14" t="s">
+    <row r="30" spans="3:6" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="C30" s="22"/>
+      <c r="D30" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="E26" s="11">
+      <c r="E30" s="11">
         <v>2</v>
       </c>
-      <c r="F26" s="12" t="s">
+      <c r="F30" s="12" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="27" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C27" s="21"/>
-      <c r="D27" s="5" t="s">
+    <row r="31" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C31" s="22"/>
+      <c r="D31" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E27" s="5">
-        <v>5</v>
-      </c>
-      <c r="F27" s="3"/>
-    </row>
-    <row r="28" spans="3:6" ht="82.5" x14ac:dyDescent="0.3">
-      <c r="C28" s="21"/>
-      <c r="D28" s="11" t="s">
+      <c r="E31" s="5">
+        <v>6</v>
+      </c>
+      <c r="F31" s="3"/>
+    </row>
+    <row r="32" spans="3:6" ht="82.5" x14ac:dyDescent="0.3">
+      <c r="C32" s="22"/>
+      <c r="D32" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="E28" s="11">
+      <c r="E32" s="11">
         <v>3</v>
       </c>
-      <c r="F28" s="12" t="s">
+      <c r="F32" s="12" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="29" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C29" s="21"/>
-      <c r="D29" s="5" t="s">
+    <row r="33" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C33" s="22"/>
+      <c r="D33" s="5" t="s">
         <v>57</v>
-      </c>
-      <c r="E29" s="5">
-        <v>5</v>
-      </c>
-      <c r="F29" s="12"/>
-    </row>
-    <row r="30" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C30" s="21"/>
-      <c r="D30" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="E30" s="5">
-        <v>5</v>
-      </c>
-      <c r="F30" s="12"/>
-    </row>
-    <row r="31" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C31" s="21"/>
-      <c r="D31" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E31" s="5">
-        <v>5</v>
-      </c>
-      <c r="F31" s="3"/>
-    </row>
-    <row r="32" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C32" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="D32" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="E32" s="11">
-        <v>4</v>
-      </c>
-      <c r="F32" s="3"/>
-    </row>
-    <row r="33" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C33" s="21"/>
-      <c r="D33" s="5" t="s">
-        <v>19</v>
       </c>
       <c r="E33" s="5">
         <v>5</v>
       </c>
-      <c r="F33" s="3"/>
+      <c r="F33" s="12"/>
     </row>
     <row r="34" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C34" s="21" t="s">
-        <v>23</v>
-      </c>
+      <c r="C34" s="22"/>
       <c r="D34" s="5" t="s">
-        <v>22</v>
+        <v>62</v>
       </c>
       <c r="E34" s="5">
-        <v>6</v>
-      </c>
-      <c r="F34" s="3"/>
+        <v>5</v>
+      </c>
+      <c r="F34" s="12"/>
     </row>
     <row r="35" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C35" s="21"/>
+      <c r="C35" s="22"/>
       <c r="D35" s="5" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="E35" s="5">
         <v>6</v>
@@ -1201,106 +1216,150 @@
       <c r="F35" s="3"/>
     </row>
     <row r="36" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C36" s="3" t="s">
+      <c r="C36" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="D36" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E36" s="11">
+        <v>4</v>
+      </c>
+      <c r="F36" s="3"/>
+    </row>
+    <row r="37" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C37" s="22"/>
+      <c r="D37" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E37" s="5">
+        <v>6</v>
+      </c>
+      <c r="F37" s="3"/>
+    </row>
+    <row r="38" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C38" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E38" s="5">
+        <v>6</v>
+      </c>
+      <c r="F38" s="3"/>
+    </row>
+    <row r="39" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C39" s="22"/>
+      <c r="D39" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E39" s="5">
+        <v>6</v>
+      </c>
+      <c r="F39" s="3"/>
+    </row>
+    <row r="40" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C40" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D36" s="5" t="s">
+      <c r="D40" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E36" s="5">
+      <c r="E40" s="5">
         <v>9</v>
       </c>
-      <c r="F36" s="3"/>
-    </row>
-    <row r="37" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C37" s="3" t="s">
+      <c r="F40" s="3"/>
+    </row>
+    <row r="41" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C41" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D37" s="5" t="s">
+      <c r="D41" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E37" s="5">
+      <c r="E41" s="5">
         <v>10</v>
       </c>
-      <c r="F37" s="3"/>
-    </row>
-    <row r="38" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C38" s="3" t="s">
+      <c r="F41" s="3"/>
+    </row>
+    <row r="42" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C42" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D38" s="5" t="s">
+      <c r="D42" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E38" s="5" t="s">
+      <c r="E42" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="F38" s="3"/>
-    </row>
-    <row r="39" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C39" s="18" t="s">
+      <c r="F42" s="3"/>
+    </row>
+    <row r="43" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C43" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="D39" s="11" t="s">
+      <c r="D43" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="E39" s="11">
+      <c r="E43" s="11">
         <v>2</v>
       </c>
-      <c r="F39" s="15" t="s">
+      <c r="F43" s="15" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="40" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C40" s="19"/>
-      <c r="D40" s="11" t="s">
+    <row r="44" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C44" s="20"/>
+      <c r="D44" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="E40" s="11">
+      <c r="E44" s="11">
         <v>2</v>
       </c>
-      <c r="F40" s="15" t="s">
+      <c r="F44" s="15" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="41" spans="3:6" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="C41" s="19"/>
-      <c r="D41" s="11" t="s">
+    <row r="45" spans="3:6" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="C45" s="20"/>
+      <c r="D45" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="E41" s="11">
+      <c r="E45" s="11">
         <v>3</v>
       </c>
-      <c r="F41" s="12" t="s">
+      <c r="F45" s="12" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="42" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C42" s="20"/>
-      <c r="D42" s="11" t="s">
+    <row r="46" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C46" s="21"/>
+      <c r="D46" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="E42" s="11">
+      <c r="E46" s="11">
         <v>3</v>
       </c>
-      <c r="F42" s="15" t="s">
+      <c r="F46" s="15" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="44" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C44" s="1" t="s">
+    <row r="48" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C48" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D44" s="16"/>
+      <c r="D48" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="C39:C42"/>
-    <mergeCell ref="C34:C35"/>
-    <mergeCell ref="C7:C16"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="C25:C31"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="C17:C22"/>
+    <mergeCell ref="C43:C46"/>
+    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="C7:C19"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="C29:C35"/>
+    <mergeCell ref="C36:C37"/>
+    <mergeCell ref="C20:C26"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Skill System - Cost mana
1. 스킬 쓰면 마나 닳도록 만듬.
(근데 구조 맘에 안들어서 리펙토링 예정)
</commit_message>
<xml_diff>
--- a/기능구현서.xlsx
+++ b/기능구현서.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="83">
   <si>
     <t>구현 내용</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -250,10 +250,6 @@
   </si>
   <si>
     <t>몬스터 사망 애니메이션 구현</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>리펙토링</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -354,6 +350,34 @@
   </si>
   <si>
     <t>플레이어 스탯과 UI 연동</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>어느정도 시간이 지나면 자원이 생성되도록</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>근데 진짜 설계 거지같이 해서 나중에 리펙토링 할 것</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>StateMachineBehaviour에 있는 멤버는 인스펙터에서 할당이 안되는걸 첨 알아따..</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>리펙토링 할 것</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>보조젬 중복 적용 안되게 태그를 통해 제한하기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>스킬 쓸 때 마나가 소모되는 구조가 굉장히 맘에 안듬</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -492,7 +516,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -550,6 +574,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -561,6 +588,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -571,8 +601,8 @@
   <colors>
     <mruColors>
       <color rgb="FFBEE395"/>
+      <color rgb="FFFF8585"/>
       <color rgb="FFFFFF65"/>
-      <color rgb="FFFF8585"/>
     </mruColors>
   </colors>
   <extLst>
@@ -849,10 +879,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C5:J48"/>
+  <dimension ref="C5:J50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -892,7 +922,7 @@
       <c r="J6" s="10"/>
     </row>
     <row r="7" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C7" s="22" t="s">
+      <c r="C7" s="23" t="s">
         <v>7</v>
       </c>
       <c r="D7" s="7" t="s">
@@ -904,7 +934,7 @@
       <c r="F7" s="3"/>
     </row>
     <row r="8" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C8" s="22"/>
+      <c r="C8" s="23"/>
       <c r="D8" s="8" t="s">
         <v>35</v>
       </c>
@@ -914,7 +944,7 @@
       <c r="F8" s="3"/>
     </row>
     <row r="9" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C9" s="22"/>
+      <c r="C9" s="23"/>
       <c r="D9" s="5" t="s">
         <v>6</v>
       </c>
@@ -924,7 +954,7 @@
       <c r="F9" s="3"/>
     </row>
     <row r="10" spans="3:10" ht="99" x14ac:dyDescent="0.3">
-      <c r="C10" s="22"/>
+      <c r="C10" s="23"/>
       <c r="D10" s="11" t="s">
         <v>37</v>
       </c>
@@ -932,11 +962,11 @@
         <v>1</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C11" s="22"/>
+      <c r="C11" s="23"/>
       <c r="D11" s="11" t="s">
         <v>38</v>
       </c>
@@ -946,7 +976,7 @@
       <c r="F11" s="12"/>
     </row>
     <row r="12" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C12" s="22"/>
+      <c r="C12" s="23"/>
       <c r="D12" s="11" t="s">
         <v>36</v>
       </c>
@@ -956,17 +986,17 @@
       <c r="F12" s="3"/>
     </row>
     <row r="13" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C13" s="22"/>
+      <c r="C13" s="23"/>
       <c r="D13" s="5" t="s">
         <v>39</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F13" s="4"/>
     </row>
     <row r="14" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C14" s="22"/>
+      <c r="C14" s="23"/>
       <c r="D14" s="14" t="s">
         <v>9</v>
       </c>
@@ -978,7 +1008,7 @@
       </c>
     </row>
     <row r="15" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C15" s="22"/>
+      <c r="C15" s="23"/>
       <c r="D15" s="14" t="s">
         <v>50</v>
       </c>
@@ -990,9 +1020,9 @@
       </c>
     </row>
     <row r="16" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C16" s="22"/>
+      <c r="C16" s="23"/>
       <c r="D16" s="14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E16" s="11">
         <v>5</v>
@@ -1000,205 +1030,209 @@
       <c r="F16" s="18"/>
     </row>
     <row r="17" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C17" s="22"/>
+      <c r="C17" s="23"/>
       <c r="D17" s="14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E17" s="11">
         <v>5</v>
       </c>
-      <c r="F17" s="18"/>
+      <c r="F17" s="19" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="18" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C18" s="22"/>
-      <c r="D18" s="14" t="s">
-        <v>75</v>
-      </c>
-      <c r="E18" s="11">
+      <c r="C18" s="23"/>
+      <c r="D18" s="24" t="s">
+        <v>76</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="F18" s="19"/>
+    </row>
+    <row r="19" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C19" s="23"/>
+      <c r="D19" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="E19" s="11">
         <v>5</v>
       </c>
-      <c r="F18" s="18"/>
-    </row>
-    <row r="19" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C19" s="22"/>
-      <c r="D19" s="6" t="s">
+      <c r="F19" s="18"/>
+    </row>
+    <row r="20" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C20" s="23"/>
+      <c r="D20" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="E19" s="5">
+      <c r="E20" s="5">
         <v>8</v>
       </c>
-      <c r="F19" s="3"/>
-    </row>
-    <row r="20" spans="3:6" ht="198" x14ac:dyDescent="0.3">
-      <c r="C20" s="19" t="s">
+      <c r="F20" s="3"/>
+    </row>
+    <row r="21" spans="3:6" ht="198" x14ac:dyDescent="0.3">
+      <c r="C21" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="D20" s="11" t="s">
+      <c r="D21" s="11" t="s">
         <v>10</v>
-      </c>
-      <c r="E20" s="11">
-        <v>4</v>
-      </c>
-      <c r="F20" s="12" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="21" spans="3:6" ht="33" x14ac:dyDescent="0.3">
-      <c r="C21" s="20"/>
-      <c r="D21" s="11" t="s">
-        <v>11</v>
       </c>
       <c r="E21" s="11">
         <v>4</v>
       </c>
       <c r="F21" s="12" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="22" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C22" s="20"/>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="22" spans="3:6" ht="33" x14ac:dyDescent="0.3">
+      <c r="C22" s="21"/>
       <c r="D22" s="11" t="s">
-        <v>61</v>
+        <v>11</v>
       </c>
       <c r="E22" s="11">
         <v>4</v>
       </c>
-      <c r="F22" s="3" t="s">
-        <v>67</v>
+      <c r="F22" s="12" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="23" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C23" s="20"/>
+      <c r="C23" s="21"/>
       <c r="D23" s="11" t="s">
-        <v>12</v>
+        <v>60</v>
       </c>
       <c r="E23" s="11">
         <v>4</v>
       </c>
-      <c r="F23" s="17"/>
-    </row>
-    <row r="24" spans="3:6" ht="66" x14ac:dyDescent="0.3">
-      <c r="C24" s="20"/>
+      <c r="F23" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="24" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C24" s="21"/>
       <c r="D24" s="11" t="s">
-        <v>68</v>
+        <v>12</v>
       </c>
       <c r="E24" s="11">
         <v>4</v>
       </c>
-      <c r="F24" s="12" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="25" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C25" s="20"/>
-      <c r="D25" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="E25" s="5">
-        <v>5</v>
-      </c>
-      <c r="F25" s="12"/>
+      <c r="F24" s="17"/>
+    </row>
+    <row r="25" spans="3:6" ht="66" x14ac:dyDescent="0.3">
+      <c r="C25" s="21"/>
+      <c r="D25" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="E25" s="11">
+        <v>4</v>
+      </c>
+      <c r="F25" s="12" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="26" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C26" s="21"/>
       <c r="D26" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="E26" s="11">
+        <v>5</v>
+      </c>
+      <c r="F26" s="12" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="27" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C27" s="22"/>
+      <c r="D27" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="E27" s="11">
+        <v>4</v>
+      </c>
+      <c r="F27" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="E26" s="11">
-        <v>4</v>
-      </c>
-      <c r="F26" s="12" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="27" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C27" s="22" t="s">
+    </row>
+    <row r="28" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C28" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="D28" s="5" t="s">
         <v>14</v>
-      </c>
-      <c r="E27" s="5">
-        <v>7</v>
-      </c>
-      <c r="F27" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="28" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C28" s="22"/>
-      <c r="D28" s="5" t="s">
-        <v>13</v>
       </c>
       <c r="E28" s="5">
         <v>7</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="29" spans="3:6" ht="33" x14ac:dyDescent="0.3">
-      <c r="C29" s="22" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="29" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C29" s="23"/>
+      <c r="D29" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E29" s="5">
+        <v>7</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="30" spans="3:6" ht="33" x14ac:dyDescent="0.3">
+      <c r="C30" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="D29" s="11" t="s">
+      <c r="D30" s="11" t="s">
         <v>41</v>
-      </c>
-      <c r="E29" s="11">
-        <v>2</v>
-      </c>
-      <c r="F29" s="12" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="30" spans="3:6" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="C30" s="22"/>
-      <c r="D30" s="14" t="s">
-        <v>42</v>
       </c>
       <c r="E30" s="11">
         <v>2</v>
       </c>
       <c r="F30" s="12" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="31" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C31" s="22"/>
-      <c r="D31" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="31" spans="3:6" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="C31" s="23"/>
+      <c r="D31" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="E31" s="11">
+        <v>2</v>
+      </c>
+      <c r="F31" s="12" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="32" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C32" s="23"/>
+      <c r="D32" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E31" s="5">
+      <c r="E32" s="5">
         <v>6</v>
       </c>
-      <c r="F31" s="3"/>
-    </row>
-    <row r="32" spans="3:6" ht="82.5" x14ac:dyDescent="0.3">
-      <c r="C32" s="22"/>
-      <c r="D32" s="11" t="s">
+      <c r="F32" s="3"/>
+    </row>
+    <row r="33" spans="3:6" ht="82.5" x14ac:dyDescent="0.3">
+      <c r="C33" s="23"/>
+      <c r="D33" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="E32" s="11">
+      <c r="E33" s="11">
         <v>3</v>
       </c>
-      <c r="F32" s="12" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="33" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C33" s="22"/>
-      <c r="D33" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="E33" s="5">
-        <v>5</v>
-      </c>
-      <c r="F33" s="12"/>
+      <c r="F33" s="12" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="34" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C34" s="22"/>
+      <c r="C34" s="23"/>
       <c r="D34" s="5" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="E34" s="5">
         <v>5</v>
@@ -1206,43 +1240,41 @@
       <c r="F34" s="12"/>
     </row>
     <row r="35" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C35" s="22"/>
+      <c r="C35" s="23"/>
       <c r="D35" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E35" s="5">
+        <v>5</v>
+      </c>
+      <c r="F35" s="12"/>
+    </row>
+    <row r="36" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C36" s="23"/>
+      <c r="D36" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E35" s="5">
+      <c r="E36" s="5">
         <v>6</v>
       </c>
-      <c r="F35" s="3"/>
-    </row>
-    <row r="36" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C36" s="22" t="s">
+      <c r="F36" s="3"/>
+    </row>
+    <row r="37" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C37" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="D36" s="14" t="s">
+      <c r="D37" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="E36" s="11">
+      <c r="E37" s="11">
         <v>4</v>
       </c>
-      <c r="F36" s="3"/>
-    </row>
-    <row r="37" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C37" s="22"/>
-      <c r="D37" s="5" t="s">
+      <c r="F37" s="3"/>
+    </row>
+    <row r="38" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C38" s="23"/>
+      <c r="D38" s="5" t="s">
         <v>19</v>
-      </c>
-      <c r="E37" s="5">
-        <v>6</v>
-      </c>
-      <c r="F37" s="3"/>
-    </row>
-    <row r="38" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C38" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="D38" s="5" t="s">
-        <v>22</v>
       </c>
       <c r="E38" s="5">
         <v>6</v>
@@ -1250,9 +1282,11 @@
       <c r="F38" s="3"/>
     </row>
     <row r="39" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C39" s="22"/>
+      <c r="C39" s="23" t="s">
+        <v>23</v>
+      </c>
       <c r="D39" s="5" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="E39" s="5">
         <v>6</v>
@@ -1260,106 +1294,123 @@
       <c r="F39" s="3"/>
     </row>
     <row r="40" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C40" s="3" t="s">
-        <v>24</v>
-      </c>
+      <c r="C40" s="23"/>
       <c r="D40" s="5" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="E40" s="5">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F40" s="3"/>
     </row>
     <row r="41" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C41" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E41" s="5">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F41" s="3"/>
     </row>
     <row r="42" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C42" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E42" s="5">
+        <v>10</v>
+      </c>
+      <c r="F42" s="3"/>
+    </row>
+    <row r="43" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C43" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D42" s="5" t="s">
+      <c r="D43" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E42" s="5" t="s">
+      <c r="E43" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="F42" s="3"/>
-    </row>
-    <row r="43" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C43" s="19" t="s">
+      <c r="F43" s="3"/>
+    </row>
+    <row r="44" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C44" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="D43" s="11" t="s">
+      <c r="D44" s="11" t="s">
         <v>45</v>
-      </c>
-      <c r="E43" s="11">
-        <v>2</v>
-      </c>
-      <c r="F43" s="15" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="44" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C44" s="20"/>
-      <c r="D44" s="11" t="s">
-        <v>46</v>
       </c>
       <c r="E44" s="11">
         <v>2</v>
       </c>
       <c r="F44" s="15" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="45" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C45" s="21"/>
+      <c r="D45" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="E45" s="11">
+        <v>2</v>
+      </c>
+      <c r="F45" s="15" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="45" spans="3:6" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="C45" s="20"/>
-      <c r="D45" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="E45" s="11">
-        <v>3</v>
-      </c>
-      <c r="F45" s="12" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="46" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="3:6" ht="49.5" x14ac:dyDescent="0.3">
       <c r="C46" s="21"/>
       <c r="D46" s="11" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="E46" s="11">
         <v>3</v>
       </c>
-      <c r="F46" s="15" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="48" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C48" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D48" s="16"/>
+      <c r="F46" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="47" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C47" s="22"/>
+      <c r="D47" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="E47" s="11">
+        <v>3</v>
+      </c>
+      <c r="F47" s="15" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="49" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C49" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D49" s="16" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="50" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="D50" s="1" t="s">
+        <v>82</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="C43:C46"/>
-    <mergeCell ref="C38:C39"/>
-    <mergeCell ref="C7:C19"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="C29:C35"/>
-    <mergeCell ref="C36:C37"/>
-    <mergeCell ref="C20:C26"/>
+    <mergeCell ref="C44:C47"/>
+    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="C7:C20"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="C30:C36"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="C21:C27"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Get Exp & Bleeding
1. 몬스터, 플레이어 모두 데미지를 받으면 피를 흘리게 바꿈

2. 몬스터 죽이면 경험치 얻도록 구현
</commit_message>
<xml_diff>
--- a/기능구현서.xlsx
+++ b/기능구현서.xlsx
@@ -253,10 +253,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>몬스터 피격 시 피 이펙트 적용</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>이건 2D 때도 했는데, 액션 리스트로 더 잘 만들어보면 됌</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -385,12 +381,16 @@
 해결) 그냥 함수 순서 조절해줌</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>몬스터 피격 시 피 이펙트 적용 및 죽으면 경험치 주도록</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -423,6 +423,14 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="맑은 고딕"/>
       <family val="3"/>
       <charset val="129"/>
@@ -521,7 +529,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -597,7 +605,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -609,8 +620,8 @@
   <colors>
     <mruColors>
       <color rgb="FFBEE395"/>
+      <color rgb="FFFF8585"/>
       <color rgb="FFFFFF65"/>
-      <color rgb="FFFF8585"/>
     </mruColors>
   </colors>
   <extLst>
@@ -890,7 +901,7 @@
   <dimension ref="C5:J50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -970,7 +981,7 @@
         <v>1</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11" spans="3:10" x14ac:dyDescent="0.3">
@@ -999,7 +1010,7 @@
         <v>39</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F13" s="4"/>
     </row>
@@ -1030,7 +1041,7 @@
     <row r="16" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C16" s="24"/>
       <c r="D16" s="14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E16" s="11">
         <v>5</v>
@@ -1040,29 +1051,29 @@
     <row r="17" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C17" s="24"/>
       <c r="D17" s="14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E17" s="11">
         <v>5</v>
       </c>
       <c r="F17" s="19" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="18" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C18" s="24"/>
       <c r="D18" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="E18" s="5" t="s">
         <v>76</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>77</v>
       </c>
       <c r="F18" s="19"/>
     </row>
     <row r="19" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C19" s="24"/>
       <c r="D19" s="14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E19" s="11">
         <v>5</v>
@@ -1090,7 +1101,7 @@
         <v>4</v>
       </c>
       <c r="F21" s="12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="22" spans="3:6" ht="33" x14ac:dyDescent="0.3">
@@ -1102,19 +1113,19 @@
         <v>4</v>
       </c>
       <c r="F22" s="12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="23" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C23" s="22"/>
       <c r="D23" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E23" s="11">
         <v>4</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="24" spans="3:6" x14ac:dyDescent="0.3">
@@ -1130,37 +1141,37 @@
     <row r="25" spans="3:6" ht="66" x14ac:dyDescent="0.3">
       <c r="C25" s="22"/>
       <c r="D25" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E25" s="11">
         <v>4</v>
       </c>
       <c r="F25" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="26" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C26" s="22"/>
       <c r="D26" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E26" s="11">
         <v>5</v>
       </c>
       <c r="F26" s="12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="27" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C27" s="23"/>
       <c r="D27" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E27" s="11">
         <v>4</v>
       </c>
       <c r="F27" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="28" spans="3:6" x14ac:dyDescent="0.3">
@@ -1186,7 +1197,7 @@
         <v>7</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="30" spans="3:6" ht="33" x14ac:dyDescent="0.3">
@@ -1212,7 +1223,7 @@
         <v>2</v>
       </c>
       <c r="F31" s="12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="32" spans="3:6" x14ac:dyDescent="0.3">
@@ -1234,15 +1245,15 @@
         <v>3</v>
       </c>
       <c r="F33" s="12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="34" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C34" s="24"/>
       <c r="D34" s="25" t="s">
-        <v>56</v>
-      </c>
-      <c r="E34" s="25">
+        <v>83</v>
+      </c>
+      <c r="E34" s="26">
         <v>5</v>
       </c>
       <c r="F34" s="12"/>
@@ -1250,13 +1261,13 @@
     <row r="35" spans="3:6" ht="33" x14ac:dyDescent="0.3">
       <c r="C35" s="24"/>
       <c r="D35" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E35" s="11">
         <v>5</v>
       </c>
       <c r="F35" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="36" spans="3:6" x14ac:dyDescent="0.3">
@@ -1396,20 +1407,20 @@
         <v>3</v>
       </c>
       <c r="F47" s="15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="49" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C49" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D49" s="16" t="s">
         <v>80</v>
-      </c>
-      <c r="D49" s="16" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="50" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D50" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Monster Random Position Spawn
몬스터가 랜덤한 위치에서 생성되게 함
</commit_message>
<xml_diff>
--- a/기능구현서.xlsx
+++ b/기능구현서.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="102">
   <si>
     <t>구현 내용</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -440,12 +440,28 @@
     <t>??</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>이동, 공격, 시전 등의 스탯이 영향을 주도록</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>몬스터 랜덤 스폰 구현</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>떨어져있는 아이템을 다시 땅바닥으로 드래그 하면 아이템이 복사되는 버그</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>떨어진 아이템을 바로 장착 시도하는 경우 아이템 옵션이 적용이 안됨</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -584,7 +600,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -673,6 +689,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -962,13 +981,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C5:J60"/>
+  <dimension ref="C5:J64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F36" activeCellId="1" sqref="D34:E34 F36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="15.875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="82.75" style="1" bestFit="1" customWidth="1"/>
@@ -976,7 +995,7 @@
     <col min="6" max="6" width="95.625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="3:10">
+    <row r="5" spans="3:10" x14ac:dyDescent="0.3">
       <c r="H5" t="s">
         <v>34</v>
       </c>
@@ -987,7 +1006,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="3:10">
+    <row r="6" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C6" s="3" t="s">
         <v>8</v>
       </c>
@@ -1004,7 +1023,7 @@
       <c r="I6" s="9"/>
       <c r="J6" s="10"/>
     </row>
-    <row r="7" spans="3:10">
+    <row r="7" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C7" s="29" t="s">
         <v>7</v>
       </c>
@@ -1016,7 +1035,7 @@
       </c>
       <c r="F7" s="3"/>
     </row>
-    <row r="8" spans="3:10">
+    <row r="8" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C8" s="29"/>
       <c r="D8" s="8" t="s">
         <v>35</v>
@@ -1026,7 +1045,7 @@
       </c>
       <c r="F8" s="3"/>
     </row>
-    <row r="9" spans="3:10">
+    <row r="9" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C9" s="29"/>
       <c r="D9" s="5" t="s">
         <v>6</v>
@@ -1036,7 +1055,7 @@
       </c>
       <c r="F9" s="3"/>
     </row>
-    <row r="10" spans="3:10" ht="99">
+    <row r="10" spans="3:10" ht="99" x14ac:dyDescent="0.3">
       <c r="C10" s="29"/>
       <c r="D10" s="11" t="s">
         <v>37</v>
@@ -1048,7 +1067,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="11" spans="3:10">
+    <row r="11" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C11" s="29"/>
       <c r="D11" s="11" t="s">
         <v>38</v>
@@ -1058,7 +1077,7 @@
       </c>
       <c r="F11" s="12"/>
     </row>
-    <row r="12" spans="3:10">
+    <row r="12" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C12" s="29"/>
       <c r="D12" s="11" t="s">
         <v>36</v>
@@ -1068,7 +1087,7 @@
       </c>
       <c r="F12" s="3"/>
     </row>
-    <row r="13" spans="3:10">
+    <row r="13" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C13" s="29"/>
       <c r="D13" s="5" t="s">
         <v>39</v>
@@ -1078,7 +1097,7 @@
       </c>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="3:10">
+    <row r="14" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C14" s="29"/>
       <c r="D14" s="14" t="s">
         <v>9</v>
@@ -1090,7 +1109,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="3:10">
+    <row r="15" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C15" s="29"/>
       <c r="D15" s="14" t="s">
         <v>50</v>
@@ -1102,7 +1121,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="16" spans="3:10">
+    <row r="16" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C16" s="29"/>
       <c r="D16" s="14" t="s">
         <v>71</v>
@@ -1112,7 +1131,7 @@
       </c>
       <c r="F16" s="18"/>
     </row>
-    <row r="17" spans="3:6">
+    <row r="17" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C17" s="29"/>
       <c r="D17" s="14" t="s">
         <v>73</v>
@@ -1124,7 +1143,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="18" spans="3:6">
+    <row r="18" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C18" s="29"/>
       <c r="D18" s="14" t="s">
         <v>74</v>
@@ -1134,7 +1153,7 @@
       </c>
       <c r="F18" s="19"/>
     </row>
-    <row r="19" spans="3:6">
+    <row r="19" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C19" s="29"/>
       <c r="D19" s="14" t="s">
         <v>72</v>
@@ -1144,7 +1163,7 @@
       </c>
       <c r="F19" s="18"/>
     </row>
-    <row r="20" spans="3:6">
+    <row r="20" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C20" s="29"/>
       <c r="D20" s="6" t="s">
         <v>29</v>
@@ -1154,7 +1173,7 @@
       </c>
       <c r="F20" s="3"/>
     </row>
-    <row r="21" spans="3:6" ht="198">
+    <row r="21" spans="3:6" ht="198" x14ac:dyDescent="0.3">
       <c r="C21" s="26" t="s">
         <v>4</v>
       </c>
@@ -1168,7 +1187,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="22" spans="3:6" ht="33">
+    <row r="22" spans="3:6" ht="33" x14ac:dyDescent="0.3">
       <c r="C22" s="27"/>
       <c r="D22" s="11" t="s">
         <v>11</v>
@@ -1180,7 +1199,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="23" spans="3:6">
+    <row r="23" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C23" s="27"/>
       <c r="D23" s="11" t="s">
         <v>58</v>
@@ -1192,7 +1211,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="24" spans="3:6">
+    <row r="24" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C24" s="27"/>
       <c r="D24" s="11" t="s">
         <v>12</v>
@@ -1202,7 +1221,7 @@
       </c>
       <c r="F24" s="17"/>
     </row>
-    <row r="25" spans="3:6" ht="66">
+    <row r="25" spans="3:6" ht="66" x14ac:dyDescent="0.3">
       <c r="C25" s="27"/>
       <c r="D25" s="11" t="s">
         <v>65</v>
@@ -1214,7 +1233,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="26" spans="3:6">
+    <row r="26" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C26" s="27"/>
       <c r="D26" s="11" t="s">
         <v>70</v>
@@ -1226,7 +1245,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="27" spans="3:6">
+    <row r="27" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C27" s="28"/>
       <c r="D27" s="11" t="s">
         <v>67</v>
@@ -1238,7 +1257,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="28" spans="3:6">
+    <row r="28" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C28" s="29" t="s">
         <v>16</v>
       </c>
@@ -1252,7 +1271,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="29" spans="3:6">
+    <row r="29" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C29" s="29"/>
       <c r="D29" s="11" t="s">
         <v>86</v>
@@ -1262,7 +1281,7 @@
       </c>
       <c r="F29" s="21"/>
     </row>
-    <row r="30" spans="3:6">
+    <row r="30" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C30" s="29"/>
       <c r="D30" s="11" t="s">
         <v>85</v>
@@ -1274,7 +1293,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="31" spans="3:6">
+    <row r="31" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C31" s="29"/>
       <c r="D31" s="11" t="s">
         <v>13</v>
@@ -1286,7 +1305,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="32" spans="3:6" ht="33">
+    <row r="32" spans="3:6" ht="33" x14ac:dyDescent="0.3">
       <c r="C32" s="29" t="s">
         <v>20</v>
       </c>
@@ -1300,7 +1319,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="33" spans="3:6" ht="49.5">
+    <row r="33" spans="3:6" ht="49.5" x14ac:dyDescent="0.3">
       <c r="C33" s="29"/>
       <c r="D33" s="14" t="s">
         <v>42</v>
@@ -1312,276 +1331,301 @@
         <v>56</v>
       </c>
     </row>
-    <row r="34" spans="3:6">
+    <row r="34" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C34" s="29"/>
-      <c r="D34" s="5" t="s">
+      <c r="D34" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="E34" s="11">
+        <v>8</v>
+      </c>
+      <c r="F34" s="12"/>
+    </row>
+    <row r="35" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C35" s="29"/>
+      <c r="D35" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="E34" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="F34" s="3"/>
-    </row>
-    <row r="35" spans="3:6" ht="82.5">
-      <c r="C35" s="29"/>
-      <c r="D35" s="11" t="s">
+      <c r="E35" s="30">
+        <v>8</v>
+      </c>
+      <c r="F35" s="3"/>
+    </row>
+    <row r="36" spans="3:6" ht="82.5" x14ac:dyDescent="0.3">
+      <c r="C36" s="29"/>
+      <c r="D36" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="E35" s="11">
+      <c r="E36" s="11">
         <v>3</v>
       </c>
-      <c r="F35" s="12" t="s">
+      <c r="F36" s="12" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="36" spans="3:6">
-      <c r="C36" s="29"/>
-      <c r="D36" s="22" t="s">
+    <row r="37" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C37" s="29"/>
+      <c r="D37" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="E36" s="23">
+      <c r="E37" s="23">
         <v>5</v>
       </c>
-      <c r="F36" s="12"/>
-    </row>
-    <row r="37" spans="3:6" ht="33">
-      <c r="C37" s="29"/>
-      <c r="D37" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="E37" s="11">
-        <v>5</v>
-      </c>
-      <c r="F37" s="12" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="38" spans="3:6">
+      <c r="F37" s="12"/>
+    </row>
+    <row r="38" spans="3:6" ht="33" x14ac:dyDescent="0.3">
       <c r="C38" s="29"/>
       <c r="D38" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="E38" s="11">
+        <v>5</v>
+      </c>
+      <c r="F38" s="12" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="39" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C39" s="29"/>
+      <c r="D39" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="E38" s="11">
+      <c r="E39" s="11">
         <v>7</v>
       </c>
-      <c r="F38" s="3"/>
-    </row>
-    <row r="39" spans="3:6">
-      <c r="C39" s="29" t="s">
+      <c r="F39" s="3"/>
+    </row>
+    <row r="40" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C40" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="D39" s="14" t="s">
+      <c r="D40" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="E39" s="11">
+      <c r="E40" s="11">
         <v>4</v>
       </c>
-      <c r="F39" s="3"/>
-    </row>
-    <row r="40" spans="3:6">
-      <c r="C40" s="29"/>
-      <c r="D40" s="20" t="s">
+      <c r="F40" s="3"/>
+    </row>
+    <row r="41" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C41" s="29"/>
+      <c r="D41" s="20" t="s">
         <v>83</v>
       </c>
-      <c r="E40" s="5" t="s">
+      <c r="E41" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="F40" s="21"/>
-    </row>
-    <row r="41" spans="3:6">
-      <c r="C41" s="29"/>
-      <c r="D41" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="E41" s="11">
-        <v>7</v>
-      </c>
       <c r="F41" s="21"/>
     </row>
-    <row r="42" spans="3:6">
+    <row r="42" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C42" s="29"/>
       <c r="D42" s="14" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="E42" s="11">
         <v>7</v>
       </c>
-      <c r="F42" s="24"/>
-    </row>
-    <row r="43" spans="3:6">
+      <c r="F42" s="21"/>
+    </row>
+    <row r="43" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C43" s="29"/>
-      <c r="D43" s="11" t="s">
-        <v>19</v>
+      <c r="D43" s="14" t="s">
+        <v>93</v>
       </c>
       <c r="E43" s="11">
         <v>7</v>
       </c>
-      <c r="F43" s="3"/>
-    </row>
-    <row r="44" spans="3:6">
-      <c r="C44" s="29" t="s">
+      <c r="F43" s="24"/>
+    </row>
+    <row r="44" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C44" s="29"/>
+      <c r="D44" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E44" s="11">
+        <v>7</v>
+      </c>
+      <c r="F44" s="3"/>
+    </row>
+    <row r="45" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C45" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="D44" s="5" t="s">
+      <c r="D45" s="5" t="s">
         <v>22</v>
-      </c>
-      <c r="E44" s="5">
-        <v>8</v>
-      </c>
-      <c r="F44" s="3"/>
-    </row>
-    <row r="45" spans="3:6">
-      <c r="C45" s="29"/>
-      <c r="D45" s="5" t="s">
-        <v>30</v>
       </c>
       <c r="E45" s="5">
         <v>8</v>
       </c>
       <c r="F45" s="3"/>
     </row>
-    <row r="46" spans="3:6">
-      <c r="C46" s="3" t="s">
+    <row r="46" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C46" s="29"/>
+      <c r="D46" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E46" s="5">
+        <v>8</v>
+      </c>
+      <c r="F46" s="3"/>
+    </row>
+    <row r="47" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C47" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D46" s="5" t="s">
+      <c r="D47" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E46" s="5" t="s">
+      <c r="E47" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="F46" s="3"/>
-    </row>
-    <row r="47" spans="3:6">
-      <c r="C47" s="3" t="s">
+      <c r="F47" s="3"/>
+    </row>
+    <row r="48" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C48" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D47" s="5" t="s">
+      <c r="D48" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E47" s="5">
+      <c r="E48" s="5">
         <v>10</v>
       </c>
-      <c r="F47" s="3"/>
-    </row>
-    <row r="48" spans="3:6">
-      <c r="C48" s="3" t="s">
+      <c r="F48" s="3"/>
+    </row>
+    <row r="49" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C49" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D48" s="5" t="s">
+      <c r="D49" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E48" s="5" t="s">
+      <c r="E49" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="F48" s="3"/>
-    </row>
-    <row r="49" spans="3:6">
-      <c r="C49" s="26" t="s">
+      <c r="F49" s="3"/>
+    </row>
+    <row r="50" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C50" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="D49" s="11" t="s">
+      <c r="D50" s="11" t="s">
         <v>45</v>
-      </c>
-      <c r="E49" s="11">
-        <v>2</v>
-      </c>
-      <c r="F49" s="15" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="50" spans="3:6">
-      <c r="C50" s="27"/>
-      <c r="D50" s="11" t="s">
-        <v>46</v>
       </c>
       <c r="E50" s="11">
         <v>2</v>
       </c>
       <c r="F50" s="15" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="51" spans="3:6" ht="49.5">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="51" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C51" s="27"/>
       <c r="D51" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="E51" s="11">
+        <v>2</v>
+      </c>
+      <c r="F51" s="15" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="52" spans="3:6" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="C52" s="27"/>
+      <c r="D52" s="11" t="s">
         <v>53</v>
-      </c>
-      <c r="E51" s="11">
-        <v>3</v>
-      </c>
-      <c r="F51" s="12" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="52" spans="3:6">
-      <c r="C52" s="28"/>
-      <c r="D52" s="11" t="s">
-        <v>49</v>
       </c>
       <c r="E52" s="11">
         <v>3</v>
       </c>
-      <c r="F52" s="15" t="s">
+      <c r="F52" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="53" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C53" s="28"/>
+      <c r="D53" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="E53" s="11">
+        <v>3</v>
+      </c>
+      <c r="F53" s="15" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="54" spans="3:6">
-      <c r="C54" s="1" t="s">
+    <row r="55" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C55" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="D54" s="16" t="s">
+      <c r="D55" s="16" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="55" spans="3:6">
-      <c r="D55" s="1" t="s">
+    <row r="56" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="D56" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="56" spans="3:6">
-      <c r="D56" s="25" t="s">
+    <row r="57" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="D57" s="25" t="s">
         <v>87</v>
-      </c>
-      <c r="E56" s="25"/>
-      <c r="F56" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="57" spans="3:6">
-      <c r="D57" s="25" t="s">
-        <v>88</v>
       </c>
       <c r="E57" s="25"/>
       <c r="F57" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="58" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="D58" s="25" t="s">
+        <v>88</v>
+      </c>
+      <c r="E58" s="25"/>
+      <c r="F58" s="1" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="58" spans="3:6">
-      <c r="D58" s="25" t="s">
+    <row r="59" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="D59" s="25" t="s">
         <v>89</v>
       </c>
-      <c r="E58" s="25"/>
-    </row>
-    <row r="59" spans="3:6">
-      <c r="D59" s="1" t="s">
+      <c r="E59" s="25"/>
+    </row>
+    <row r="60" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="D60" s="1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="60" spans="3:6">
-      <c r="D60" s="25" t="s">
+    <row r="61" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="D61" s="25" t="s">
         <v>96</v>
       </c>
-      <c r="E60" s="25"/>
+      <c r="E61" s="25"/>
+    </row>
+    <row r="62" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="D62" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="63" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="D63" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="64" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="D64" s="1" t="s">
+        <v>101</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="C49:C52"/>
-    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="C50:C53"/>
+    <mergeCell ref="C45:C46"/>
     <mergeCell ref="C7:C20"/>
     <mergeCell ref="C28:C31"/>
-    <mergeCell ref="C32:C38"/>
-    <mergeCell ref="C39:C43"/>
+    <mergeCell ref="C32:C39"/>
+    <mergeCell ref="C40:C44"/>
     <mergeCell ref="C21:C27"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Monster Pack & Gold
1. 몬스터가 팩 단위로 등장하게 함

2. 몬스터가 골드를 떨구고 플레이어가 줍고 저장할 수 있게 함
</commit_message>
<xml_diff>
--- a/기능구현서.xlsx
+++ b/기능구현서.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="108">
   <si>
     <t>구현 내용</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -454,6 +454,30 @@
   </si>
   <si>
     <t>떨어진 아이템을 바로 장착 시도하는 경우 아이템 옵션이 적용이 안됨</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>몬스터의 등급을 만들고 등급에 따라 더 좋은 아이템을 떨구도록 해보기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>??</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>??</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>플레이어 사망 판정 넣기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아이템 옵션 수치 조정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>골드를 줍고 저장할 수 있게 구현</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -679,6 +703,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -689,9 +716,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -703,8 +727,8 @@
   <colors>
     <mruColors>
       <color rgb="FFBEE395"/>
+      <color rgb="FFFF8585"/>
       <color rgb="FFFFFF65"/>
-      <color rgb="FFFF8585"/>
     </mruColors>
   </colors>
   <extLst>
@@ -981,10 +1005,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C5:J64"/>
+  <dimension ref="C5:J68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F36" activeCellId="1" sqref="D34:E34 F36"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1024,7 +1048,7 @@
       <c r="J6" s="10"/>
     </row>
     <row r="7" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C7" s="29" t="s">
+      <c r="C7" s="30" t="s">
         <v>7</v>
       </c>
       <c r="D7" s="7" t="s">
@@ -1036,7 +1060,7 @@
       <c r="F7" s="3"/>
     </row>
     <row r="8" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C8" s="29"/>
+      <c r="C8" s="30"/>
       <c r="D8" s="8" t="s">
         <v>35</v>
       </c>
@@ -1046,17 +1070,17 @@
       <c r="F8" s="3"/>
     </row>
     <row r="9" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C9" s="29"/>
+      <c r="C9" s="30"/>
       <c r="D9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="5">
-        <v>8</v>
+      <c r="E9" s="5" t="s">
+        <v>104</v>
       </c>
       <c r="F9" s="3"/>
     </row>
     <row r="10" spans="3:10" ht="99" x14ac:dyDescent="0.3">
-      <c r="C10" s="29"/>
+      <c r="C10" s="30"/>
       <c r="D10" s="11" t="s">
         <v>37</v>
       </c>
@@ -1068,7 +1092,7 @@
       </c>
     </row>
     <row r="11" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C11" s="29"/>
+      <c r="C11" s="30"/>
       <c r="D11" s="11" t="s">
         <v>38</v>
       </c>
@@ -1078,7 +1102,7 @@
       <c r="F11" s="12"/>
     </row>
     <row r="12" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C12" s="29"/>
+      <c r="C12" s="30"/>
       <c r="D12" s="11" t="s">
         <v>36</v>
       </c>
@@ -1088,7 +1112,7 @@
       <c r="F12" s="3"/>
     </row>
     <row r="13" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C13" s="29"/>
+      <c r="C13" s="30"/>
       <c r="D13" s="5" t="s">
         <v>39</v>
       </c>
@@ -1098,535 +1122,570 @@
       <c r="F13" s="4"/>
     </row>
     <row r="14" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C14" s="29"/>
-      <c r="D14" s="14" t="s">
+      <c r="C14" s="30"/>
+      <c r="D14" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="E14" s="5">
         <v>9</v>
       </c>
-      <c r="E14" s="11">
+      <c r="F14" s="26"/>
+    </row>
+    <row r="15" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C15" s="30"/>
+      <c r="D15" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" s="11">
         <v>1</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="F15" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C15" s="29"/>
-      <c r="D15" s="14" t="s">
+    <row r="16" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C16" s="30"/>
+      <c r="D16" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="E15" s="11">
+      <c r="E16" s="11">
         <v>3</v>
       </c>
-      <c r="F15" s="13" t="s">
+      <c r="F16" s="13" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="16" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C16" s="29"/>
-      <c r="D16" s="14" t="s">
+    <row r="17" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C17" s="30"/>
+      <c r="D17" s="14" t="s">
         <v>71</v>
-      </c>
-      <c r="E16" s="11">
-        <v>5</v>
-      </c>
-      <c r="F16" s="18"/>
-    </row>
-    <row r="17" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C17" s="29"/>
-      <c r="D17" s="14" t="s">
-        <v>73</v>
       </c>
       <c r="E17" s="11">
         <v>5</v>
       </c>
-      <c r="F17" s="19" t="s">
+      <c r="F17" s="18"/>
+    </row>
+    <row r="18" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C18" s="30"/>
+      <c r="D18" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="E18" s="11">
+        <v>5</v>
+      </c>
+      <c r="F18" s="19" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="18" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C18" s="29"/>
-      <c r="D18" s="14" t="s">
+    <row r="19" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C19" s="30"/>
+      <c r="D19" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="E18" s="11">
+      <c r="E19" s="11">
         <v>6</v>
       </c>
-      <c r="F18" s="19"/>
-    </row>
-    <row r="19" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C19" s="29"/>
-      <c r="D19" s="14" t="s">
+      <c r="F19" s="19"/>
+    </row>
+    <row r="20" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C20" s="30"/>
+      <c r="D20" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="E20" s="11">
+        <v>8</v>
+      </c>
+      <c r="F20" s="26"/>
+    </row>
+    <row r="21" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C21" s="30"/>
+      <c r="D21" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="E19" s="11">
+      <c r="E21" s="11">
         <v>5</v>
       </c>
-      <c r="F19" s="18"/>
-    </row>
-    <row r="20" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C20" s="29"/>
-      <c r="D20" s="6" t="s">
+      <c r="F21" s="18"/>
+    </row>
+    <row r="22" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C22" s="30"/>
+      <c r="D22" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="E20" s="5">
-        <v>8</v>
-      </c>
-      <c r="F20" s="3"/>
-    </row>
-    <row r="21" spans="3:6" ht="198" x14ac:dyDescent="0.3">
-      <c r="C21" s="26" t="s">
+      <c r="E22" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="F22" s="3"/>
+    </row>
+    <row r="23" spans="3:6" ht="198" x14ac:dyDescent="0.3">
+      <c r="C23" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="D21" s="11" t="s">
+      <c r="D23" s="11" t="s">
         <v>10</v>
-      </c>
-      <c r="E21" s="11">
-        <v>4</v>
-      </c>
-      <c r="F21" s="12" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="22" spans="3:6" ht="33" x14ac:dyDescent="0.3">
-      <c r="C22" s="27"/>
-      <c r="D22" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E22" s="11">
-        <v>4</v>
-      </c>
-      <c r="F22" s="12" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="23" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C23" s="27"/>
-      <c r="D23" s="11" t="s">
-        <v>58</v>
       </c>
       <c r="E23" s="11">
         <v>4</v>
       </c>
-      <c r="F23" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="24" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C24" s="27"/>
+      <c r="F23" s="12" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="24" spans="3:6" ht="33" x14ac:dyDescent="0.3">
+      <c r="C24" s="28"/>
       <c r="D24" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E24" s="11">
         <v>4</v>
       </c>
-      <c r="F24" s="17"/>
-    </row>
-    <row r="25" spans="3:6" ht="66" x14ac:dyDescent="0.3">
-      <c r="C25" s="27"/>
+      <c r="F24" s="12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="25" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C25" s="28"/>
       <c r="D25" s="11" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="E25" s="11">
         <v>4</v>
       </c>
-      <c r="F25" s="12" t="s">
-        <v>66</v>
+      <c r="F25" s="3" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="26" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C26" s="27"/>
+      <c r="C26" s="28"/>
       <c r="D26" s="11" t="s">
-        <v>70</v>
+        <v>12</v>
       </c>
       <c r="E26" s="11">
-        <v>5</v>
-      </c>
-      <c r="F26" s="12" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="27" spans="3:6" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+      <c r="F26" s="17"/>
+    </row>
+    <row r="27" spans="3:6" ht="66" x14ac:dyDescent="0.3">
       <c r="C27" s="28"/>
       <c r="D27" s="11" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E27" s="11">
         <v>4</v>
       </c>
       <c r="F27" s="12" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="28" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C28" s="29" t="s">
-        <v>16</v>
-      </c>
+      <c r="C28" s="28"/>
       <c r="D28" s="11" t="s">
-        <v>14</v>
+        <v>70</v>
       </c>
       <c r="E28" s="11">
-        <v>6</v>
-      </c>
-      <c r="F28" s="3" t="s">
-        <v>52</v>
+        <v>5</v>
+      </c>
+      <c r="F28" s="12" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="29" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C29" s="29"/>
       <c r="D29" s="11" t="s">
-        <v>86</v>
+        <v>67</v>
       </c>
       <c r="E29" s="11">
-        <v>6</v>
-      </c>
-      <c r="F29" s="21"/>
+        <v>4</v>
+      </c>
+      <c r="F29" s="12" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="30" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C30" s="29"/>
+      <c r="C30" s="30" t="s">
+        <v>16</v>
+      </c>
       <c r="D30" s="11" t="s">
-        <v>85</v>
+        <v>14</v>
       </c>
       <c r="E30" s="11">
         <v>6</v>
       </c>
-      <c r="F30" s="21" t="s">
-        <v>92</v>
+      <c r="F30" s="3" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="31" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C31" s="29"/>
+      <c r="C31" s="30"/>
       <c r="D31" s="11" t="s">
-        <v>13</v>
+        <v>86</v>
       </c>
       <c r="E31" s="11">
         <v>6</v>
       </c>
-      <c r="F31" s="3" t="s">
+      <c r="F31" s="21"/>
+    </row>
+    <row r="32" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C32" s="30"/>
+      <c r="D32" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="E32" s="11">
+        <v>6</v>
+      </c>
+      <c r="F32" s="21" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="33" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C33" s="30"/>
+      <c r="D33" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E33" s="11">
+        <v>6</v>
+      </c>
+      <c r="F33" s="3" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="32" spans="3:6" ht="33" x14ac:dyDescent="0.3">
-      <c r="C32" s="29" t="s">
+    <row r="34" spans="3:6" ht="33" x14ac:dyDescent="0.3">
+      <c r="C34" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="D32" s="11" t="s">
+      <c r="D34" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="E32" s="11">
+      <c r="E34" s="11">
         <v>2</v>
       </c>
-      <c r="F32" s="12" t="s">
+      <c r="F34" s="12" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="33" spans="3:6" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="C33" s="29"/>
-      <c r="D33" s="14" t="s">
+    <row r="35" spans="3:6" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="C35" s="30"/>
+      <c r="D35" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="E33" s="11">
+      <c r="E35" s="11">
         <v>2</v>
       </c>
-      <c r="F33" s="12" t="s">
+      <c r="F35" s="12" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="34" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C34" s="29"/>
-      <c r="D34" s="14" t="s">
+    <row r="36" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C36" s="30"/>
+      <c r="D36" s="14" t="s">
         <v>99</v>
       </c>
-      <c r="E34" s="11">
+      <c r="E36" s="11">
         <v>8</v>
       </c>
-      <c r="F34" s="12"/>
-    </row>
-    <row r="35" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C35" s="29"/>
-      <c r="D35" s="30" t="s">
+      <c r="F36" s="12"/>
+    </row>
+    <row r="37" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C37" s="30"/>
+      <c r="D37" s="20" t="s">
+        <v>102</v>
+      </c>
+      <c r="E37" s="5">
+        <v>9</v>
+      </c>
+      <c r="F37" s="12"/>
+    </row>
+    <row r="38" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C38" s="30"/>
+      <c r="D38" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="E35" s="30">
+      <c r="E38" s="11">
         <v>8</v>
       </c>
-      <c r="F35" s="3"/>
-    </row>
-    <row r="36" spans="3:6" ht="82.5" x14ac:dyDescent="0.3">
-      <c r="C36" s="29"/>
-      <c r="D36" s="11" t="s">
+      <c r="F38" s="3"/>
+    </row>
+    <row r="39" spans="3:6" ht="82.5" x14ac:dyDescent="0.3">
+      <c r="C39" s="30"/>
+      <c r="D39" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="E36" s="11">
+      <c r="E39" s="11">
         <v>3</v>
       </c>
-      <c r="F36" s="12" t="s">
+      <c r="F39" s="12" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="37" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C37" s="29"/>
-      <c r="D37" s="22" t="s">
+    <row r="40" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C40" s="30"/>
+      <c r="D40" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="E37" s="23">
+      <c r="E40" s="23">
         <v>5</v>
       </c>
-      <c r="F37" s="12"/>
-    </row>
-    <row r="38" spans="3:6" ht="33" x14ac:dyDescent="0.3">
-      <c r="C38" s="29"/>
-      <c r="D38" s="11" t="s">
+      <c r="F40" s="12"/>
+    </row>
+    <row r="41" spans="3:6" ht="33" x14ac:dyDescent="0.3">
+      <c r="C41" s="30"/>
+      <c r="D41" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="E38" s="11">
+      <c r="E41" s="11">
         <v>5</v>
       </c>
-      <c r="F38" s="12" t="s">
+      <c r="F41" s="12" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="39" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C39" s="29"/>
-      <c r="D39" s="11" t="s">
+    <row r="42" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C42" s="30"/>
+      <c r="D42" s="11" t="s">
         <v>18</v>
-      </c>
-      <c r="E39" s="11">
-        <v>7</v>
-      </c>
-      <c r="F39" s="3"/>
-    </row>
-    <row r="40" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C40" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="D40" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="E40" s="11">
-        <v>4</v>
-      </c>
-      <c r="F40" s="3"/>
-    </row>
-    <row r="41" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C41" s="29"/>
-      <c r="D41" s="20" t="s">
-        <v>83</v>
-      </c>
-      <c r="E41" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="F41" s="21"/>
-    </row>
-    <row r="42" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C42" s="29"/>
-      <c r="D42" s="14" t="s">
-        <v>82</v>
       </c>
       <c r="E42" s="11">
         <v>7</v>
       </c>
-      <c r="F42" s="21"/>
+      <c r="F42" s="3"/>
     </row>
     <row r="43" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C43" s="29"/>
+      <c r="C43" s="30" t="s">
+        <v>21</v>
+      </c>
       <c r="D43" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E43" s="11">
+        <v>4</v>
+      </c>
+      <c r="F43" s="3"/>
+    </row>
+    <row r="44" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C44" s="30"/>
+      <c r="D44" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="E44" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="F44" s="21"/>
+    </row>
+    <row r="45" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C45" s="30"/>
+      <c r="D45" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="E45" s="11">
+        <v>7</v>
+      </c>
+      <c r="F45" s="21"/>
+    </row>
+    <row r="46" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C46" s="30"/>
+      <c r="D46" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="E43" s="11">
+      <c r="E46" s="11">
         <v>7</v>
       </c>
-      <c r="F43" s="24"/>
-    </row>
-    <row r="44" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C44" s="29"/>
-      <c r="D44" s="11" t="s">
+      <c r="F46" s="24"/>
+    </row>
+    <row r="47" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C47" s="30"/>
+      <c r="D47" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="E44" s="11">
+      <c r="E47" s="11">
         <v>7</v>
       </c>
-      <c r="F44" s="3"/>
-    </row>
-    <row r="45" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C45" s="29" t="s">
+      <c r="F47" s="3"/>
+    </row>
+    <row r="48" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C48" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="D45" s="5" t="s">
+      <c r="D48" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E45" s="5">
+      <c r="E48" s="5">
         <v>8</v>
       </c>
-      <c r="F45" s="3"/>
-    </row>
-    <row r="46" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C46" s="29"/>
-      <c r="D46" s="5" t="s">
+      <c r="F48" s="3"/>
+    </row>
+    <row r="49" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C49" s="30"/>
+      <c r="D49" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="E46" s="5">
+      <c r="E49" s="5">
         <v>8</v>
       </c>
-      <c r="F46" s="3"/>
-    </row>
-    <row r="47" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C47" s="3" t="s">
+      <c r="F49" s="3"/>
+    </row>
+    <row r="50" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C50" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D47" s="5" t="s">
+      <c r="D50" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E47" s="5" t="s">
+      <c r="E50" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="F47" s="3"/>
-    </row>
-    <row r="48" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C48" s="3" t="s">
+      <c r="F50" s="3"/>
+    </row>
+    <row r="51" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C51" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D48" s="5" t="s">
+      <c r="D51" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E48" s="5">
+      <c r="E51" s="5">
         <v>10</v>
       </c>
-      <c r="F48" s="3"/>
-    </row>
-    <row r="49" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C49" s="3" t="s">
+      <c r="F51" s="3"/>
+    </row>
+    <row r="52" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C52" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D49" s="5" t="s">
+      <c r="D52" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E49" s="5" t="s">
+      <c r="E52" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="F49" s="3"/>
-    </row>
-    <row r="50" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C50" s="26" t="s">
+      <c r="F52" s="3"/>
+    </row>
+    <row r="53" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C53" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="D50" s="11" t="s">
+      <c r="D53" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="E50" s="11">
+      <c r="E53" s="11">
         <v>2</v>
       </c>
-      <c r="F50" s="15" t="s">
+      <c r="F53" s="15" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="51" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C51" s="27"/>
-      <c r="D51" s="11" t="s">
+    <row r="54" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C54" s="28"/>
+      <c r="D54" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="E51" s="11">
+      <c r="E54" s="11">
         <v>2</v>
       </c>
-      <c r="F51" s="15" t="s">
+      <c r="F54" s="15" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="52" spans="3:6" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="C52" s="27"/>
-      <c r="D52" s="11" t="s">
+    <row r="55" spans="3:6" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="C55" s="28"/>
+      <c r="D55" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="E52" s="11">
+      <c r="E55" s="11">
         <v>3</v>
       </c>
-      <c r="F52" s="12" t="s">
+      <c r="F55" s="12" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="53" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C53" s="28"/>
-      <c r="D53" s="11" t="s">
+    <row r="56" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C56" s="29"/>
+      <c r="D56" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="E53" s="11">
+      <c r="E56" s="11">
         <v>3</v>
       </c>
-      <c r="F53" s="15" t="s">
+      <c r="F56" s="15" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="55" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C55" s="1" t="s">
+    <row r="58" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C58" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="D55" s="16" t="s">
+      <c r="D58" s="16" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="56" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="D56" s="1" t="s">
+    <row r="59" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="D59" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="57" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="D57" s="25" t="s">
+    <row r="60" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="D60" s="25" t="s">
         <v>87</v>
       </c>
-      <c r="E57" s="25"/>
-      <c r="F57" s="1" t="s">
+      <c r="E60" s="25"/>
+      <c r="F60" s="1" t="s">
         <v>90</v>
-      </c>
-    </row>
-    <row r="58" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="D58" s="25" t="s">
-        <v>88</v>
-      </c>
-      <c r="E58" s="25"/>
-      <c r="F58" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="59" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="D59" s="25" t="s">
-        <v>89</v>
-      </c>
-      <c r="E59" s="25"/>
-    </row>
-    <row r="60" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="D60" s="1" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="61" spans="3:6" x14ac:dyDescent="0.3">
       <c r="D61" s="25" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="E61" s="25"/>
+      <c r="F61" s="1" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="62" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="D62" s="1" t="s">
-        <v>98</v>
-      </c>
+      <c r="D62" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="E62" s="25"/>
     </row>
     <row r="63" spans="3:6" x14ac:dyDescent="0.3">
       <c r="D63" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="64" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="D64" s="25" t="s">
+        <v>96</v>
+      </c>
+      <c r="E64" s="25"/>
+    </row>
+    <row r="65" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D65" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="66" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D66" s="1" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="64" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="D64" s="1" t="s">
+    <row r="67" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D67" s="1" t="s">
         <v>101</v>
+      </c>
+    </row>
+    <row r="68" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D68" s="1" t="s">
+        <v>106</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="C50:C53"/>
-    <mergeCell ref="C45:C46"/>
-    <mergeCell ref="C7:C20"/>
-    <mergeCell ref="C28:C31"/>
-    <mergeCell ref="C32:C39"/>
-    <mergeCell ref="C40:C44"/>
-    <mergeCell ref="C21:C27"/>
+    <mergeCell ref="C53:C56"/>
+    <mergeCell ref="C48:C49"/>
+    <mergeCell ref="C7:C22"/>
+    <mergeCell ref="C30:C33"/>
+    <mergeCell ref="C34:C42"/>
+    <mergeCell ref="C43:C47"/>
+    <mergeCell ref="C23:C29"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>